<commit_message>
entered result for cse 101 sec 8 and mat 101 section 4
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 101/results_cse101_sec9.xlsx
+++ b/FALL 19/CSE 101/results_cse101_sec9.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\CSE 101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{708842B0-E63C-4D66-A52C-CC2D22DA1DC7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFF7ECF-F590-4505-91AB-9CB439EA0F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quiz1" sheetId="1" r:id="rId1"/>
     <sheet name="quiz2" sheetId="3" r:id="rId2"/>
     <sheet name="quiz_final" sheetId="4" r:id="rId3"/>
     <sheet name="mid" sheetId="2" r:id="rId4"/>
+    <sheet name="final" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="67">
   <si>
     <t>ID</t>
   </si>
@@ -227,12 +228,18 @@
   <si>
     <t>Quiz_Converted</t>
   </si>
+  <si>
+    <t>Problem 5</t>
+  </si>
+  <si>
+    <t>Marks 5</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -280,6 +287,10 @@
       <color rgb="FF000000"/>
       <name val="Cambria"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -330,7 +341,47 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -6421,17 +6472,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G48">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6444,7 +6495,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92239A0-A3FC-4ACB-BB8E-9DDF5BDE05CE}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I2" sqref="I2:J48"/>
     </sheetView>
   </sheetViews>
@@ -8101,12 +8152,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9718,8 +9769,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11894,26 +11945,2181 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G48">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="2" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485E7955-23DA-41EB-BFE8-1A0365DA72E9}">
+  <dimension ref="A1:P48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="16" width="14.77734375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="4">
+        <v>173011011</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5">
+        <v>5</v>
+      </c>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5">
+        <v>5</v>
+      </c>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5">
+        <v>10</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5">
+        <v>10</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5">
+        <v>10</v>
+      </c>
+      <c r="M2" s="6">
+        <f>C2+E2+G2+I2+K2</f>
+        <v>0</v>
+      </c>
+      <c r="N2" s="6">
+        <f>D2+F2+H2+J2+L2</f>
+        <v>40</v>
+      </c>
+      <c r="O2" s="10">
+        <f>(M2/N2)*100</f>
+        <v>0</v>
+      </c>
+      <c r="P2" s="11" t="str">
+        <f>IF(O2&gt;94,"A+",IF(O2&gt;84,"A",IF(O2&gt;79,"A-",IF(O2&gt;74,"B+",IF(O2&gt;69,"B",IF(O2&gt;64,"B-",IF(O2&gt;59,"C+",IF(O2&gt;54,"C",IF(O2&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="4">
+        <v>181014084</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="5">
+        <v>5</v>
+      </c>
+      <c r="E3" s="7"/>
+      <c r="F3" s="5">
+        <v>5</v>
+      </c>
+      <c r="G3" s="7"/>
+      <c r="H3" s="5">
+        <v>10</v>
+      </c>
+      <c r="I3" s="7"/>
+      <c r="J3" s="5">
+        <v>10</v>
+      </c>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5">
+        <v>10</v>
+      </c>
+      <c r="M3" s="6">
+        <f>C3+E3+G3+I3</f>
+        <v>0</v>
+      </c>
+      <c r="N3" s="6">
+        <f t="shared" ref="N3:N48" si="0">D3+F3+H3+J3+L3</f>
+        <v>40</v>
+      </c>
+      <c r="O3" s="10">
+        <f t="shared" ref="O3:O48" si="1">(M3/N3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="11" t="str">
+        <f t="shared" ref="P3:P48" si="2">IF(O3&gt;94,"A+",IF(O3&gt;84,"A",IF(O3&gt;79,"A-",IF(O3&gt;74,"B+",IF(O3&gt;69,"B",IF(O3&gt;64,"B-",IF(O3&gt;59,"C+",IF(O3&gt;54,"C",IF(O3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="4">
+        <v>183011124</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5">
+        <v>5</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5">
+        <v>10</v>
+      </c>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5">
+        <v>10</v>
+      </c>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5">
+        <v>10</v>
+      </c>
+      <c r="M4" s="6">
+        <f>C4+E4+G4+I4</f>
+        <v>0</v>
+      </c>
+      <c r="N4" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O4" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="4">
+        <v>183013056</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5">
+        <v>5</v>
+      </c>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5">
+        <v>5</v>
+      </c>
+      <c r="G5" s="5"/>
+      <c r="H5" s="5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5">
+        <v>10</v>
+      </c>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5">
+        <v>10</v>
+      </c>
+      <c r="M5" s="6">
+        <f>C5+E5+G5+I5</f>
+        <v>0</v>
+      </c>
+      <c r="N5" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O5" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P5" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="4">
+        <v>183013064</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="7"/>
+      <c r="F6" s="5">
+        <v>5</v>
+      </c>
+      <c r="G6" s="7"/>
+      <c r="H6" s="5">
+        <v>10</v>
+      </c>
+      <c r="I6" s="7"/>
+      <c r="J6" s="5">
+        <v>10</v>
+      </c>
+      <c r="K6" s="5"/>
+      <c r="L6" s="5">
+        <v>10</v>
+      </c>
+      <c r="M6" s="6">
+        <f>C6+E6+G6+I6</f>
+        <v>0</v>
+      </c>
+      <c r="N6" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O6" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P6" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="4">
+        <v>183014013</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5">
+        <v>5</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5">
+        <v>10</v>
+      </c>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5">
+        <v>10</v>
+      </c>
+      <c r="K7" s="5"/>
+      <c r="L7" s="5">
+        <v>10</v>
+      </c>
+      <c r="M7" s="6">
+        <f>C7+E7+G7+I7</f>
+        <v>0</v>
+      </c>
+      <c r="N7" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O7" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P7" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="4">
+        <v>183014047</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5">
+        <v>5</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5">
+        <v>10</v>
+      </c>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5">
+        <v>10</v>
+      </c>
+      <c r="K8" s="5"/>
+      <c r="L8" s="5">
+        <v>10</v>
+      </c>
+      <c r="M8" s="6">
+        <f>C8+E8+G8+I8</f>
+        <v>0</v>
+      </c>
+      <c r="N8" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O8" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="4">
+        <v>183014061</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="7"/>
+      <c r="F9" s="5">
+        <v>5</v>
+      </c>
+      <c r="G9" s="7"/>
+      <c r="H9" s="5">
+        <v>10</v>
+      </c>
+      <c r="I9" s="7"/>
+      <c r="J9" s="5">
+        <v>10</v>
+      </c>
+      <c r="K9" s="5"/>
+      <c r="L9" s="5">
+        <v>10</v>
+      </c>
+      <c r="M9" s="6">
+        <f>C9+E9+G9+I9</f>
+        <v>0</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O9" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P9" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="4">
+        <v>191011024</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5">
+        <v>5</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5">
+        <v>10</v>
+      </c>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5">
+        <v>10</v>
+      </c>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5">
+        <v>10</v>
+      </c>
+      <c r="M10" s="6">
+        <f>C10+E10+G10+I10</f>
+        <v>0</v>
+      </c>
+      <c r="N10" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O10" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P10" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="4">
+        <v>191014023</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5">
+        <v>5</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5">
+        <v>10</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5">
+        <v>10</v>
+      </c>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5">
+        <v>10</v>
+      </c>
+      <c r="M11" s="6">
+        <f>C11+E11+G11+I11</f>
+        <v>0</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O11" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="4">
+        <v>191014032</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
+        <v>5</v>
+      </c>
+      <c r="H12" s="5">
+        <v>10</v>
+      </c>
+      <c r="J12" s="5">
+        <v>10</v>
+      </c>
+      <c r="K12" s="5"/>
+      <c r="L12" s="5">
+        <v>10</v>
+      </c>
+      <c r="M12" s="6">
+        <f>C12+E12+G12+I12</f>
+        <v>0</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O12" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P12" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="4">
+        <v>191014069</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+      <c r="E13" s="7"/>
+      <c r="F13" s="5">
+        <v>5</v>
+      </c>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5">
+        <v>10</v>
+      </c>
+      <c r="I13" s="7"/>
+      <c r="J13" s="5">
+        <v>10</v>
+      </c>
+      <c r="K13" s="5"/>
+      <c r="L13" s="5">
+        <v>10</v>
+      </c>
+      <c r="M13" s="6">
+        <f>C13+E13+G13+I13</f>
+        <v>0</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O13" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P13" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="4">
+        <v>192011115</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="5"/>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5">
+        <v>5</v>
+      </c>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5">
+        <v>10</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5">
+        <v>10</v>
+      </c>
+      <c r="K14" s="5"/>
+      <c r="L14" s="5">
+        <v>10</v>
+      </c>
+      <c r="M14" s="6">
+        <f>C14+E14+G14+I14</f>
+        <v>0</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O14" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="4">
+        <v>192014019</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5">
+        <v>5</v>
+      </c>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5">
+        <v>10</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5">
+        <v>10</v>
+      </c>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5">
+        <v>10</v>
+      </c>
+      <c r="M15" s="6">
+        <f>C15+E15+G15+I15</f>
+        <v>0</v>
+      </c>
+      <c r="N15" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O15" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P15" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="4">
+        <v>192014023</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="7"/>
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+      <c r="E16" s="7"/>
+      <c r="F16" s="5">
+        <v>5</v>
+      </c>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5">
+        <v>10</v>
+      </c>
+      <c r="I16" s="7"/>
+      <c r="J16" s="5">
+        <v>10</v>
+      </c>
+      <c r="K16" s="5"/>
+      <c r="L16" s="5">
+        <v>10</v>
+      </c>
+      <c r="M16" s="6">
+        <f>C16+E16+G16+I16</f>
+        <v>0</v>
+      </c>
+      <c r="N16" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O16" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P16" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="4">
+        <v>192014029</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5">
+        <v>5</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5">
+        <v>10</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5">
+        <v>10</v>
+      </c>
+      <c r="K17" s="5"/>
+      <c r="L17" s="5">
+        <v>10</v>
+      </c>
+      <c r="M17" s="6">
+        <f>C17+E17+G17+I17</f>
+        <v>0</v>
+      </c>
+      <c r="N17" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O17" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P17" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="4">
+        <v>193011030</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="7"/>
+      <c r="D18" s="5">
+        <v>5</v>
+      </c>
+      <c r="E18" s="7"/>
+      <c r="F18" s="5">
+        <v>5</v>
+      </c>
+      <c r="G18" s="7"/>
+      <c r="H18" s="5">
+        <v>10</v>
+      </c>
+      <c r="I18" s="7"/>
+      <c r="J18" s="5">
+        <v>10</v>
+      </c>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5">
+        <v>10</v>
+      </c>
+      <c r="M18" s="6">
+        <f>C18+E18+G18+I18</f>
+        <v>0</v>
+      </c>
+      <c r="N18" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O18" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P18" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="4">
+        <v>193012069</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5">
+        <v>5</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5">
+        <v>10</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5">
+        <v>10</v>
+      </c>
+      <c r="K19" s="5"/>
+      <c r="L19" s="5">
+        <v>10</v>
+      </c>
+      <c r="M19" s="6">
+        <f>C19+E19+G19+I19</f>
+        <v>0</v>
+      </c>
+      <c r="N19" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O19" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="4">
+        <v>193014003</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5">
+        <v>5</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5">
+        <v>10</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5">
+        <v>10</v>
+      </c>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5">
+        <v>10</v>
+      </c>
+      <c r="M20" s="6">
+        <f>C20+E20+G20+I20</f>
+        <v>0</v>
+      </c>
+      <c r="N20" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O20" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P20" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="4">
+        <v>193014005</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="5"/>
+      <c r="D21" s="5">
+        <v>5</v>
+      </c>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5">
+        <v>5</v>
+      </c>
+      <c r="G21" s="5"/>
+      <c r="H21" s="5">
+        <v>10</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="J21" s="5">
+        <v>10</v>
+      </c>
+      <c r="K21" s="5"/>
+      <c r="L21" s="5">
+        <v>10</v>
+      </c>
+      <c r="M21" s="6">
+        <f>C21+E21+G21+I21</f>
+        <v>0</v>
+      </c>
+      <c r="N21" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O21" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P21" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="4">
+        <v>193014007</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="5"/>
+      <c r="D22" s="5">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5">
+        <v>5</v>
+      </c>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5">
+        <v>10</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="J22" s="5">
+        <v>10</v>
+      </c>
+      <c r="K22" s="5"/>
+      <c r="L22" s="5">
+        <v>10</v>
+      </c>
+      <c r="M22" s="6">
+        <f>C22+E22+G22+I22</f>
+        <v>0</v>
+      </c>
+      <c r="N22" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O22" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P22" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="4">
+        <v>193014009</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5">
+        <v>5</v>
+      </c>
+      <c r="G23" s="5"/>
+      <c r="H23" s="5">
+        <v>10</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="J23" s="5">
+        <v>10</v>
+      </c>
+      <c r="K23" s="5"/>
+      <c r="L23" s="5">
+        <v>10</v>
+      </c>
+      <c r="M23" s="6">
+        <f>C23+E23+G23+I23</f>
+        <v>0</v>
+      </c>
+      <c r="N23" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O23" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P23" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="4">
+        <v>193014010</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5">
+        <v>5</v>
+      </c>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5">
+        <v>5</v>
+      </c>
+      <c r="G24" s="5"/>
+      <c r="H24" s="5">
+        <v>10</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="J24" s="5">
+        <v>10</v>
+      </c>
+      <c r="K24" s="5"/>
+      <c r="L24" s="5">
+        <v>10</v>
+      </c>
+      <c r="M24" s="6">
+        <f>C24+E24+G24+I24</f>
+        <v>0</v>
+      </c>
+      <c r="N24" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O24" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P24" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="4">
+        <v>193014015</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="7"/>
+      <c r="D25" s="5">
+        <v>5</v>
+      </c>
+      <c r="E25" s="7"/>
+      <c r="F25" s="5">
+        <v>5</v>
+      </c>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5">
+        <v>10</v>
+      </c>
+      <c r="I25" s="7"/>
+      <c r="J25" s="5">
+        <v>10</v>
+      </c>
+      <c r="K25" s="5"/>
+      <c r="L25" s="5">
+        <v>10</v>
+      </c>
+      <c r="M25" s="6">
+        <f>C25+E25+G25+I25</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O25" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P25" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="4">
+        <v>193014016</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="7"/>
+      <c r="D26" s="5">
+        <v>5</v>
+      </c>
+      <c r="E26" s="7"/>
+      <c r="F26" s="5">
+        <v>5</v>
+      </c>
+      <c r="G26" s="7"/>
+      <c r="H26" s="5">
+        <v>10</v>
+      </c>
+      <c r="I26" s="7"/>
+      <c r="J26" s="5">
+        <v>10</v>
+      </c>
+      <c r="K26" s="5"/>
+      <c r="L26" s="5">
+        <v>10</v>
+      </c>
+      <c r="M26" s="6">
+        <f>C26+E26+G26+I26</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O26" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P26" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="4">
+        <v>193014019</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5">
+        <v>5</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="5">
+        <v>10</v>
+      </c>
+      <c r="I27" s="5"/>
+      <c r="J27" s="5">
+        <v>10</v>
+      </c>
+      <c r="K27" s="5"/>
+      <c r="L27" s="5">
+        <v>10</v>
+      </c>
+      <c r="M27" s="6">
+        <f>C27+E27+G27+I27</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O27" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P27" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="4">
+        <v>193014026</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5">
+        <v>5</v>
+      </c>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5">
+        <v>10</v>
+      </c>
+      <c r="I28" s="5"/>
+      <c r="J28" s="5">
+        <v>10</v>
+      </c>
+      <c r="K28" s="5"/>
+      <c r="L28" s="5">
+        <v>10</v>
+      </c>
+      <c r="M28" s="6">
+        <f>C28+E28+G28+I28</f>
+        <v>0</v>
+      </c>
+      <c r="N28" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O28" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="4">
+        <v>193014030</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5">
+        <v>5</v>
+      </c>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5">
+        <v>5</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5">
+        <v>10</v>
+      </c>
+      <c r="I29" s="5"/>
+      <c r="J29" s="5">
+        <v>10</v>
+      </c>
+      <c r="K29" s="5"/>
+      <c r="L29" s="5">
+        <v>10</v>
+      </c>
+      <c r="M29" s="6">
+        <f>C29+E29+G29+I29</f>
+        <v>0</v>
+      </c>
+      <c r="N29" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O29" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="4">
+        <v>193014032</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="7"/>
+      <c r="D30" s="5">
+        <v>5</v>
+      </c>
+      <c r="E30" s="7"/>
+      <c r="F30" s="5">
+        <v>5</v>
+      </c>
+      <c r="G30" s="7"/>
+      <c r="H30" s="5">
+        <v>10</v>
+      </c>
+      <c r="I30" s="7"/>
+      <c r="J30" s="5">
+        <v>10</v>
+      </c>
+      <c r="K30" s="5"/>
+      <c r="L30" s="5">
+        <v>10</v>
+      </c>
+      <c r="M30" s="6">
+        <f>C30+E30+G30+I30</f>
+        <v>0</v>
+      </c>
+      <c r="N30" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O30" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P30" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="4">
+        <v>193014033</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5">
+        <v>5</v>
+      </c>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5">
+        <v>5</v>
+      </c>
+      <c r="G31" s="5"/>
+      <c r="H31" s="5">
+        <v>10</v>
+      </c>
+      <c r="I31" s="5"/>
+      <c r="J31" s="5">
+        <v>10</v>
+      </c>
+      <c r="K31" s="5"/>
+      <c r="L31" s="5">
+        <v>10</v>
+      </c>
+      <c r="M31" s="6">
+        <f>C31+E31+G31+I31</f>
+        <v>0</v>
+      </c>
+      <c r="N31" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O31" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P31" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="4">
+        <v>193014035</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5">
+        <v>5</v>
+      </c>
+      <c r="G32" s="5"/>
+      <c r="H32" s="5">
+        <v>10</v>
+      </c>
+      <c r="I32" s="5"/>
+      <c r="J32" s="5">
+        <v>10</v>
+      </c>
+      <c r="K32" s="5"/>
+      <c r="L32" s="5">
+        <v>10</v>
+      </c>
+      <c r="M32" s="6">
+        <f>C32+E32+G32+I32</f>
+        <v>0</v>
+      </c>
+      <c r="N32" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O32" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P32" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="4">
+        <v>193014036</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="5"/>
+      <c r="D33" s="5">
+        <v>5</v>
+      </c>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5">
+        <v>5</v>
+      </c>
+      <c r="G33" s="5"/>
+      <c r="H33" s="5">
+        <v>10</v>
+      </c>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5">
+        <v>10</v>
+      </c>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5">
+        <v>10</v>
+      </c>
+      <c r="M33" s="6">
+        <f>C33+E33+G33+I33</f>
+        <v>0</v>
+      </c>
+      <c r="N33" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O33" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P33" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="4">
+        <v>193014040</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5">
+        <v>5</v>
+      </c>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5">
+        <v>5</v>
+      </c>
+      <c r="G34" s="5"/>
+      <c r="H34" s="5">
+        <v>10</v>
+      </c>
+      <c r="I34" s="5"/>
+      <c r="J34" s="5">
+        <v>10</v>
+      </c>
+      <c r="K34" s="5"/>
+      <c r="L34" s="5">
+        <v>10</v>
+      </c>
+      <c r="M34" s="6">
+        <f>C34+E34+G34+I34</f>
+        <v>0</v>
+      </c>
+      <c r="N34" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O34" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P34" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="4">
+        <v>193014042</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5">
+        <v>5</v>
+      </c>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5">
+        <v>5</v>
+      </c>
+      <c r="G35" s="5"/>
+      <c r="H35" s="5">
+        <v>10</v>
+      </c>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5">
+        <v>10</v>
+      </c>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5">
+        <v>10</v>
+      </c>
+      <c r="M35" s="6">
+        <f>C35+E35+G35+I35</f>
+        <v>0</v>
+      </c>
+      <c r="N35" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O35" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="4">
+        <v>193014048</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5">
+        <v>5</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5">
+        <v>5</v>
+      </c>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5">
+        <v>10</v>
+      </c>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5">
+        <v>10</v>
+      </c>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5">
+        <v>10</v>
+      </c>
+      <c r="M36" s="6">
+        <f>C36+E36+G36+I36</f>
+        <v>0</v>
+      </c>
+      <c r="N36" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O36" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P36" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="4">
+        <v>193014050</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="5"/>
+      <c r="D37" s="5">
+        <v>5</v>
+      </c>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5">
+        <v>5</v>
+      </c>
+      <c r="G37" s="5"/>
+      <c r="H37" s="5">
+        <v>10</v>
+      </c>
+      <c r="I37" s="5"/>
+      <c r="J37" s="5">
+        <v>10</v>
+      </c>
+      <c r="K37" s="5"/>
+      <c r="L37" s="5">
+        <v>10</v>
+      </c>
+      <c r="M37" s="6">
+        <f>C37+E37+G37+I37</f>
+        <v>0</v>
+      </c>
+      <c r="N37" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O37" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P37" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="4">
+        <v>193014052</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5">
+        <v>5</v>
+      </c>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5">
+        <v>5</v>
+      </c>
+      <c r="G38" s="5"/>
+      <c r="H38" s="5">
+        <v>10</v>
+      </c>
+      <c r="I38" s="5"/>
+      <c r="J38" s="5">
+        <v>10</v>
+      </c>
+      <c r="K38" s="5"/>
+      <c r="L38" s="5">
+        <v>10</v>
+      </c>
+      <c r="M38" s="6">
+        <f>C38+E38+G38+I38</f>
+        <v>0</v>
+      </c>
+      <c r="N38" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O38" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P38" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="4">
+        <v>193014053</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="5"/>
+      <c r="D39" s="5">
+        <v>5</v>
+      </c>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5">
+        <v>5</v>
+      </c>
+      <c r="G39" s="5"/>
+      <c r="H39" s="5">
+        <v>10</v>
+      </c>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5">
+        <v>10</v>
+      </c>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5">
+        <v>10</v>
+      </c>
+      <c r="M39" s="6">
+        <f>C39+E39+G39+I39</f>
+        <v>0</v>
+      </c>
+      <c r="N39" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O39" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P39" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="4">
+        <v>193014055</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="5"/>
+      <c r="D40" s="5">
+        <v>5</v>
+      </c>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5">
+        <v>5</v>
+      </c>
+      <c r="G40" s="5"/>
+      <c r="H40" s="5">
+        <v>10</v>
+      </c>
+      <c r="I40" s="5"/>
+      <c r="J40" s="5">
+        <v>10</v>
+      </c>
+      <c r="K40" s="5"/>
+      <c r="L40" s="5">
+        <v>10</v>
+      </c>
+      <c r="M40" s="6">
+        <f>C40+E40+G40+I40</f>
+        <v>0</v>
+      </c>
+      <c r="N40" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O40" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P40" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="4">
+        <v>193014056</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5">
+        <v>5</v>
+      </c>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5">
+        <v>5</v>
+      </c>
+      <c r="G41" s="5"/>
+      <c r="H41" s="5">
+        <v>10</v>
+      </c>
+      <c r="I41" s="5"/>
+      <c r="J41" s="5">
+        <v>10</v>
+      </c>
+      <c r="K41" s="5"/>
+      <c r="L41" s="5">
+        <v>10</v>
+      </c>
+      <c r="M41" s="6">
+        <f>C41+E41+G41+I41</f>
+        <v>0</v>
+      </c>
+      <c r="N41" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O41" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="4">
+        <v>193014060</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5">
+        <v>5</v>
+      </c>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5">
+        <v>5</v>
+      </c>
+      <c r="G42" s="5"/>
+      <c r="H42" s="5">
+        <v>10</v>
+      </c>
+      <c r="I42" s="5"/>
+      <c r="J42" s="5">
+        <v>10</v>
+      </c>
+      <c r="K42" s="5"/>
+      <c r="L42" s="5">
+        <v>10</v>
+      </c>
+      <c r="M42" s="6">
+        <f>C42+E42+G42+I42</f>
+        <v>0</v>
+      </c>
+      <c r="N42" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O42" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P42" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="4">
+        <v>193014061</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5">
+        <v>5</v>
+      </c>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5">
+        <v>5</v>
+      </c>
+      <c r="G43" s="5"/>
+      <c r="H43" s="5">
+        <v>10</v>
+      </c>
+      <c r="I43" s="5"/>
+      <c r="J43" s="5">
+        <v>10</v>
+      </c>
+      <c r="K43" s="5"/>
+      <c r="L43" s="5">
+        <v>10</v>
+      </c>
+      <c r="M43" s="6">
+        <f>C43+E43+G43+I43</f>
+        <v>0</v>
+      </c>
+      <c r="N43" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O43" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="4">
+        <v>193014062</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5">
+        <v>5</v>
+      </c>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5">
+        <v>5</v>
+      </c>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5">
+        <v>10</v>
+      </c>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5">
+        <v>10</v>
+      </c>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5">
+        <v>10</v>
+      </c>
+      <c r="M44" s="6">
+        <f>C44+E44+G44+I44</f>
+        <v>0</v>
+      </c>
+      <c r="N44" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O44" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P44" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="4">
+        <v>193014064</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5">
+        <v>5</v>
+      </c>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5">
+        <v>5</v>
+      </c>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5">
+        <v>10</v>
+      </c>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5">
+        <v>10</v>
+      </c>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5">
+        <v>10</v>
+      </c>
+      <c r="M45" s="6">
+        <f>C45+E45+G45+I45</f>
+        <v>0</v>
+      </c>
+      <c r="N45" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O45" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P45" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="4">
+        <v>193014065</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5">
+        <v>5</v>
+      </c>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5">
+        <v>5</v>
+      </c>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5">
+        <v>10</v>
+      </c>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5">
+        <v>10</v>
+      </c>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5">
+        <v>10</v>
+      </c>
+      <c r="M46" s="6">
+        <f>C46+E46+G46+I46</f>
+        <v>0</v>
+      </c>
+      <c r="N46" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O46" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P46" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="4">
+        <v>193014067</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5">
+        <v>5</v>
+      </c>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
+        <v>5</v>
+      </c>
+      <c r="G47" s="5"/>
+      <c r="H47" s="5">
+        <v>10</v>
+      </c>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5">
+        <v>10</v>
+      </c>
+      <c r="K47" s="5"/>
+      <c r="L47" s="5">
+        <v>10</v>
+      </c>
+      <c r="M47" s="6">
+        <f>C47+E47+G47+I47</f>
+        <v>0</v>
+      </c>
+      <c r="N47" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O47" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P47" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A48" s="4">
+        <v>193014069</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5">
+        <v>5</v>
+      </c>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5">
+        <v>5</v>
+      </c>
+      <c r="G48" s="5"/>
+      <c r="H48" s="5">
+        <v>10</v>
+      </c>
+      <c r="I48" s="5"/>
+      <c r="J48" s="5">
+        <v>10</v>
+      </c>
+      <c r="K48" s="5"/>
+      <c r="L48" s="5">
+        <v>10</v>
+      </c>
+      <c r="M48" s="6">
+        <f>C48+E48+G48+I48</f>
+        <v>0</v>
+      </c>
+      <c r="N48" s="6">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="O48" s="10">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="11" t="str">
+        <f t="shared" si="2"/>
+        <v>F</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <conditionalFormatting sqref="I2:I48">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+      <formula>$J$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C2:C48">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>$D$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E48">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="greaterThan">
+      <formula>$F$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G2:G48">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+      <formula>$H$2</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added final and quiz 2 marks for cse 104 section 1, cse 208 section 1 & 2. also changed formatting of result of cse 101 section 9
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 101/results_cse101_sec9.xlsx
+++ b/FALL 19/CSE 101/results_cse101_sec9.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ulab_course_materials\FALL 19\CSE 101\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDFF7ECF-F590-4505-91AB-9CB439EA0F7E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6680B009-555D-47F7-965D-CA8616ED5428}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="quiz1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Quiz 2</t>
   </si>
   <si>
-    <t>Quiz_Total</t>
-  </si>
-  <si>
     <t>Quiz_Converted</t>
   </si>
   <si>
@@ -233,6 +230,18 @@
   </si>
   <si>
     <t>Marks 5</t>
+  </si>
+  <si>
+    <t>Total 2</t>
+  </si>
+  <si>
+    <t>Total 1</t>
+  </si>
+  <si>
+    <t>Quiz</t>
+  </si>
+  <si>
+    <t>Converted_Total</t>
   </si>
 </sst>
 </file>
@@ -301,7 +310,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -309,11 +318,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -337,6 +426,49 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -688,8 +820,8 @@
   </sheetPr>
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:I48"/>
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -2616,44 +2748,44 @@
         <v>A</v>
       </c>
     </row>
-    <row r="48" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:12" s="19" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="13">
         <v>193014069</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5">
-        <v>0</v>
-      </c>
-      <c r="D48" s="5">
-        <v>8</v>
-      </c>
-      <c r="E48" s="5">
-        <v>0</v>
-      </c>
-      <c r="F48" s="5">
+      <c r="C48" s="15">
+        <v>0</v>
+      </c>
+      <c r="D48" s="15">
+        <v>8</v>
+      </c>
+      <c r="E48" s="15">
+        <v>0</v>
+      </c>
+      <c r="F48" s="15">
         <v>12</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="15">
         <v>4</v>
       </c>
-      <c r="H48" s="5">
-        <v>10</v>
-      </c>
-      <c r="I48" s="6">
+      <c r="H48" s="15">
+        <v>10</v>
+      </c>
+      <c r="I48" s="16">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="J48" s="6">
+      <c r="J48" s="16">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="K48" s="12">
+      <c r="K48" s="17">
         <f t="shared" si="2"/>
         <v>13.333333333333334</v>
       </c>
-      <c r="L48" s="11" t="str">
+      <c r="L48" s="18" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -6495,8 +6627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A92239A0-A3FC-4ACB-BB8E-9DDF5BDE05CE}">
   <dimension ref="A1:J48"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2:J48"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -8114,38 +8246,38 @@
         <v>F</v>
       </c>
     </row>
-    <row r="48" spans="1:10" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:10" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="13">
         <v>193014069</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="15">
         <v>9.5</v>
       </c>
-      <c r="D48" s="5">
+      <c r="D48" s="15">
         <v>12</v>
       </c>
-      <c r="E48" s="5">
-        <v>8</v>
-      </c>
-      <c r="F48" s="5">
-        <v>8</v>
-      </c>
-      <c r="G48" s="6">
+      <c r="E48" s="15">
+        <v>8</v>
+      </c>
+      <c r="F48" s="15">
+        <v>8</v>
+      </c>
+      <c r="G48" s="16">
         <f t="shared" si="0"/>
         <v>17.5</v>
       </c>
-      <c r="H48" s="6">
+      <c r="H48" s="16">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="I48" s="12">
+      <c r="I48" s="17">
         <f t="shared" si="2"/>
         <v>87.5</v>
       </c>
-      <c r="J48" s="11" t="str">
+      <c r="J48" s="18" t="str">
         <f t="shared" si="3"/>
         <v>A</v>
       </c>
@@ -8167,1600 +8299,2080 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{85CB4B1B-76CD-4F9E-9206-C09FB7E3E154}">
-  <dimension ref="A1:I48"/>
+  <dimension ref="A1:L48"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="O14" sqref="O14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" customWidth="1"/>
-    <col min="2" max="2" width="30.6640625" customWidth="1"/>
-    <col min="3" max="9" width="14.6640625" customWidth="1"/>
+    <col min="1" max="1" width="14.77734375" customWidth="1"/>
+    <col min="2" max="2" width="30.77734375" customWidth="1"/>
+    <col min="3" max="12" width="14.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="23" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="H1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I1" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="K1" s="23" t="s">
         <v>55</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="24" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A2" s="25">
         <v>173011011</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="27">
         <v>27</v>
       </c>
-      <c r="D2" s="6">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <f>C2+D2</f>
+      <c r="D2" s="27">
+        <v>30</v>
+      </c>
+      <c r="E2" s="27">
+        <v>0</v>
+      </c>
+      <c r="F2" s="27">
+        <v>20</v>
+      </c>
+      <c r="G2" s="28">
+        <f>C2+E2</f>
         <v>27</v>
       </c>
-      <c r="F2">
-        <f>E2/5</f>
+      <c r="H2" s="28">
+        <f>D2+F2</f>
+        <v>50</v>
+      </c>
+      <c r="I2" s="28">
+        <f>(G2/H2)*J2</f>
         <v>5.4</v>
       </c>
-      <c r="G2">
-        <v>10</v>
-      </c>
-      <c r="H2" s="10">
-        <f>(F2/G2)*100</f>
+      <c r="J2" s="28">
+        <v>10</v>
+      </c>
+      <c r="K2" s="29">
+        <f>(I2/J2)*100</f>
         <v>54</v>
       </c>
-      <c r="I2" s="11" t="str">
-        <f>IF(H2&gt;94,"A+",IF(H2&gt;84,"A",IF(H2&gt;79,"A-",IF(H2&gt;74,"B+",IF(H2&gt;69,"B",IF(H2&gt;64,"B-",IF(H2&gt;59,"C+",IF(H2&gt;54,"C",IF(H2&gt;49,"D","F")))))))))</f>
+      <c r="L2" s="30" t="str">
+        <f>IF(K2&gt;94,"A+",IF(K2&gt;84,"A",IF(K2&gt;79,"A-",IF(K2&gt;74,"B+",IF(K2&gt;69,"B",IF(K2&gt;64,"B-",IF(K2&gt;59,"C+",IF(K2&gt;54,"C",IF(K2&gt;49,"D","F")))))))))</f>
         <v>D</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A3" s="4">
+    <row r="3" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
         <v>181014084</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E48" si="0">C3+D3</f>
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F48" si="1">E3/5</f>
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" s="10">
-        <f t="shared" ref="H3:H48" si="2">(F3/G3)*100</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="11" t="str">
-        <f t="shared" ref="I3:I48" si="3">IF(H3&gt;94,"A+",IF(H3&gt;84,"A",IF(H3&gt;79,"A-",IF(H3&gt;74,"B+",IF(H3&gt;69,"B",IF(H3&gt;64,"B-",IF(H3&gt;59,"C+",IF(H3&gt;54,"C",IF(H3&gt;49,"D","F")))))))))</f>
+      <c r="C3" s="27">
+        <v>0</v>
+      </c>
+      <c r="D3" s="27">
+        <v>30</v>
+      </c>
+      <c r="E3" s="27">
+        <v>0</v>
+      </c>
+      <c r="F3" s="27">
+        <v>20</v>
+      </c>
+      <c r="G3" s="28">
+        <f t="shared" ref="G3:G48" si="0">C3+E3</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="28">
+        <f t="shared" ref="H3:H48" si="1">D3+F3</f>
+        <v>50</v>
+      </c>
+      <c r="I3" s="28">
+        <f t="shared" ref="I3:I48" si="2">(G3/H3)*J3</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="28">
+        <v>10</v>
+      </c>
+      <c r="K3" s="29">
+        <f t="shared" ref="K3:K48" si="3">(I3/J3)*100</f>
+        <v>0</v>
+      </c>
+      <c r="L3" s="30" t="str">
+        <f t="shared" ref="L3:L48" si="4">IF(K3&gt;94,"A+",IF(K3&gt;84,"A",IF(K3&gt;79,"A-",IF(K3&gt;74,"B+",IF(K3&gt;69,"B",IF(K3&gt;64,"B-",IF(K3&gt;59,"C+",IF(K3&gt;54,"C",IF(K3&gt;49,"D","F")))))))))</f>
         <v>F</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A4" s="4">
+    <row r="4" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A4" s="25">
         <v>183011124</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="27">
         <v>28</v>
       </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4">
+      <c r="D4" s="27">
+        <v>30</v>
+      </c>
+      <c r="E4" s="27">
+        <v>0</v>
+      </c>
+      <c r="F4" s="27">
+        <v>20</v>
+      </c>
+      <c r="G4" s="28">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="F4">
-        <f t="shared" si="1"/>
-        <v>5.6</v>
-      </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" s="12">
-        <f t="shared" si="2"/>
-        <v>55.999999999999993</v>
-      </c>
-      <c r="I4" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="H4" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I4" s="28">
+        <f t="shared" si="2"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="J4" s="28">
+        <v>10</v>
+      </c>
+      <c r="K4" s="31">
+        <f t="shared" si="3"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="L4" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A5" s="4">
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A5" s="25">
         <v>183013056</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="27">
         <v>25</v>
       </c>
-      <c r="D5" s="6">
-        <v>0</v>
-      </c>
-      <c r="E5">
+      <c r="D5" s="27">
+        <v>30</v>
+      </c>
+      <c r="E5" s="27">
+        <v>0</v>
+      </c>
+      <c r="F5" s="27">
+        <v>20</v>
+      </c>
+      <c r="G5" s="28">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="F5">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5" s="12">
-        <f t="shared" si="2"/>
+      <c r="H5" s="28">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I5" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="I5" s="28">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J5" s="28">
+        <v>10</v>
+      </c>
+      <c r="K5" s="31">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="L5" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>D</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A6" s="4">
+    <row r="6" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A6" s="25">
         <v>183013064</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="6">
-        <v>0</v>
-      </c>
-      <c r="D6" s="6">
-        <v>0</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I6" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="B6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="27">
+        <v>0</v>
+      </c>
+      <c r="D6" s="27">
+        <v>30</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0</v>
+      </c>
+      <c r="F6" s="27">
+        <v>20</v>
+      </c>
+      <c r="G6" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I6" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J6" s="28">
+        <v>10</v>
+      </c>
+      <c r="K6" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L6" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="4">
+    <row r="7" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A7" s="25">
         <v>183014013</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="27">
         <v>16</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="27">
+        <v>30</v>
+      </c>
+      <c r="E7" s="27">
         <v>17</v>
       </c>
-      <c r="E7">
+      <c r="F7" s="27">
+        <v>20</v>
+      </c>
+      <c r="G7" s="28">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="F7">
-        <f t="shared" si="1"/>
-        <v>6.6</v>
-      </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7" s="12">
-        <f t="shared" si="2"/>
-        <v>65.999999999999986</v>
-      </c>
-      <c r="I7" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="H7" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I7" s="28">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="J7" s="28">
+        <v>10</v>
+      </c>
+      <c r="K7" s="31">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="L7" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="4">
+    <row r="8" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A8" s="25">
         <v>183014047</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="27">
         <v>30</v>
       </c>
-      <c r="D8" s="6">
-        <v>10</v>
-      </c>
-      <c r="E8">
+      <c r="D8" s="27">
+        <v>30</v>
+      </c>
+      <c r="E8" s="27">
+        <v>10</v>
+      </c>
+      <c r="F8" s="27">
+        <v>20</v>
+      </c>
+      <c r="G8" s="28">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F8">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8" s="10">
-        <f t="shared" si="2"/>
+      <c r="H8" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I8" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J8" s="28">
+        <v>10</v>
+      </c>
+      <c r="K8" s="29">
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="I8" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L8" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="4">
+    <row r="9" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="25">
         <v>183014061</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="6">
-        <v>0</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
-      <c r="H9" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I9" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C9" s="27">
+        <v>0</v>
+      </c>
+      <c r="D9" s="27">
+        <v>30</v>
+      </c>
+      <c r="E9" s="27">
+        <v>0</v>
+      </c>
+      <c r="F9" s="27">
+        <v>20</v>
+      </c>
+      <c r="G9" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I9" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="28">
+        <v>10</v>
+      </c>
+      <c r="K9" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L9" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A10" s="4">
+    <row r="10" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A10" s="25">
         <v>191011024</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="26" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="27">
         <v>18.5</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="27">
+        <v>30</v>
+      </c>
+      <c r="E10" s="27">
         <v>9</v>
       </c>
-      <c r="E10">
+      <c r="F10" s="27">
+        <v>20</v>
+      </c>
+      <c r="G10" s="28">
         <f t="shared" si="0"/>
         <v>27.5</v>
       </c>
-      <c r="F10">
-        <f t="shared" si="1"/>
+      <c r="H10" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I10" s="28">
+        <f t="shared" si="2"/>
         <v>5.5</v>
       </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10" s="12">
-        <f t="shared" si="2"/>
+      <c r="J10" s="28">
+        <v>10</v>
+      </c>
+      <c r="K10" s="31">
+        <f t="shared" si="3"/>
         <v>55.000000000000007</v>
       </c>
-      <c r="I10" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L10" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A11" s="4">
+    <row r="11" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
         <v>191014023</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="27">
         <v>20.5</v>
       </c>
-      <c r="D11" s="6">
-        <v>10</v>
-      </c>
-      <c r="E11">
+      <c r="D11" s="27">
+        <v>30</v>
+      </c>
+      <c r="E11" s="27">
+        <v>10</v>
+      </c>
+      <c r="F11" s="27">
+        <v>20</v>
+      </c>
+      <c r="G11" s="28">
         <f t="shared" si="0"/>
         <v>30.5</v>
       </c>
-      <c r="F11">
-        <f t="shared" si="1"/>
+      <c r="H11" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I11" s="28">
+        <f t="shared" si="2"/>
         <v>6.1</v>
       </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="H11" s="12">
-        <f t="shared" si="2"/>
+      <c r="J11" s="28">
+        <v>10</v>
+      </c>
+      <c r="K11" s="31">
+        <f t="shared" si="3"/>
         <v>61</v>
       </c>
-      <c r="I11" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L11" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A12" s="4">
+    <row r="12" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
         <v>191014032</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="26" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C12" s="27">
+        <v>0</v>
+      </c>
+      <c r="D12" s="27">
+        <v>30</v>
+      </c>
+      <c r="E12" s="27">
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <v>20</v>
+      </c>
+      <c r="G12" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I12" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J12" s="28">
+        <v>10</v>
+      </c>
+      <c r="K12" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L12" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A13" s="4">
+    <row r="13" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
         <v>191014069</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="6">
-        <v>8</v>
-      </c>
-      <c r="D13" s="6">
+      <c r="C13" s="27">
+        <v>8</v>
+      </c>
+      <c r="D13" s="27">
+        <v>30</v>
+      </c>
+      <c r="E13" s="27">
         <v>11</v>
       </c>
-      <c r="E13">
+      <c r="F13" s="27">
+        <v>20</v>
+      </c>
+      <c r="G13" s="28">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="F13">
-        <f t="shared" si="1"/>
+      <c r="H13" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I13" s="28">
+        <f t="shared" si="2"/>
         <v>3.8</v>
       </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-      <c r="H13" s="12">
-        <f t="shared" si="2"/>
+      <c r="J13" s="28">
+        <v>10</v>
+      </c>
+      <c r="K13" s="31">
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
-      <c r="I13" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L13" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A14" s="4">
+    <row r="14" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
         <v>192011115</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="27">
         <v>6</v>
       </c>
-      <c r="D14" s="6">
-        <v>0</v>
-      </c>
-      <c r="E14">
+      <c r="D14" s="27">
+        <v>30</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0</v>
+      </c>
+      <c r="F14" s="27">
+        <v>20</v>
+      </c>
+      <c r="G14" s="28">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="F14">
-        <f t="shared" si="1"/>
+      <c r="H14" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I14" s="28">
+        <f t="shared" si="2"/>
         <v>1.2</v>
       </c>
-      <c r="G14">
-        <v>10</v>
-      </c>
-      <c r="H14" s="10">
-        <f t="shared" si="2"/>
+      <c r="J14" s="28">
+        <v>10</v>
+      </c>
+      <c r="K14" s="29">
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
-      <c r="I14" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L14" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="15" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A15" s="4">
+    <row r="15" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
         <v>192014019</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="26" t="s">
         <v>19</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="27">
         <v>27</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="27">
+        <v>30</v>
+      </c>
+      <c r="E15" s="27">
         <v>17</v>
       </c>
-      <c r="E15">
+      <c r="F15" s="27">
+        <v>20</v>
+      </c>
+      <c r="G15" s="28">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="F15">
-        <f t="shared" si="1"/>
+      <c r="H15" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I15" s="28">
+        <f t="shared" si="2"/>
         <v>8.8000000000000007</v>
       </c>
-      <c r="G15">
-        <v>10</v>
-      </c>
-      <c r="H15" s="10">
-        <f t="shared" si="2"/>
+      <c r="J15" s="28">
+        <v>10</v>
+      </c>
+      <c r="K15" s="29">
+        <f t="shared" si="3"/>
         <v>88.000000000000014</v>
       </c>
-      <c r="I15" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L15" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A16" s="4">
+    <row r="16" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
         <v>192014023</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C16" s="6">
-        <v>0</v>
-      </c>
-      <c r="D16" s="6">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="H16" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I16" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C16" s="27">
+        <v>0</v>
+      </c>
+      <c r="D16" s="27">
+        <v>30</v>
+      </c>
+      <c r="E16" s="27">
+        <v>0</v>
+      </c>
+      <c r="F16" s="27">
+        <v>20</v>
+      </c>
+      <c r="G16" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H16" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I16" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="28">
+        <v>10</v>
+      </c>
+      <c r="K16" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L16" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="17" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A17" s="4">
+    <row r="17" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
         <v>192014029</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="C17" s="6">
+      <c r="C17" s="27">
         <v>23</v>
       </c>
-      <c r="D17" s="6">
+      <c r="D17" s="27">
+        <v>30</v>
+      </c>
+      <c r="E17" s="27">
         <v>17</v>
       </c>
-      <c r="E17">
+      <c r="F17" s="27">
+        <v>20</v>
+      </c>
+      <c r="G17" s="28">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F17">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17" s="12">
-        <f t="shared" si="2"/>
+      <c r="H17" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I17" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J17" s="28">
+        <v>10</v>
+      </c>
+      <c r="K17" s="31">
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="I17" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L17" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A18" s="4">
+    <row r="18" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="25">
         <v>193011030</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="6">
-        <v>0</v>
-      </c>
-      <c r="D18" s="6">
-        <v>0</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="H18" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I18" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C18" s="27">
+        <v>0</v>
+      </c>
+      <c r="D18" s="27">
+        <v>30</v>
+      </c>
+      <c r="E18" s="27">
+        <v>0</v>
+      </c>
+      <c r="F18" s="27">
+        <v>20</v>
+      </c>
+      <c r="G18" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I18" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J18" s="28">
+        <v>10</v>
+      </c>
+      <c r="K18" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L18" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A19" s="4">
+    <row r="19" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="25">
         <v>193012069</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="26" t="s">
         <v>23</v>
       </c>
-      <c r="C19" s="6">
-        <v>5</v>
-      </c>
-      <c r="D19" s="6">
-        <v>0</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="1"/>
+      <c r="C19" s="27">
+        <v>5</v>
+      </c>
+      <c r="D19" s="27">
+        <v>30</v>
+      </c>
+      <c r="E19" s="27">
+        <v>0</v>
+      </c>
+      <c r="F19" s="27">
+        <v>20</v>
+      </c>
+      <c r="G19" s="28">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="H19" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I19" s="28">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="H19" s="12">
-        <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="I19" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="J19" s="28">
+        <v>10</v>
+      </c>
+      <c r="K19" s="31">
+        <f t="shared" si="3"/>
+        <v>10</v>
+      </c>
+      <c r="L19" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A20" s="4">
+    <row r="20" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="25">
         <v>193014003</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="26" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="6">
+      <c r="C20" s="27">
         <v>28</v>
       </c>
-      <c r="D20" s="6">
+      <c r="D20" s="27">
+        <v>30</v>
+      </c>
+      <c r="E20" s="27">
         <v>18.5</v>
       </c>
-      <c r="E20">
+      <c r="F20" s="27">
+        <v>20</v>
+      </c>
+      <c r="G20" s="28">
         <f t="shared" si="0"/>
         <v>46.5</v>
       </c>
-      <c r="F20">
-        <f t="shared" si="1"/>
+      <c r="H20" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I20" s="28">
+        <f t="shared" si="2"/>
         <v>9.3000000000000007</v>
       </c>
-      <c r="G20">
-        <v>10</v>
-      </c>
-      <c r="H20" s="12">
-        <f t="shared" si="2"/>
+      <c r="J20" s="28">
+        <v>10</v>
+      </c>
+      <c r="K20" s="31">
+        <f t="shared" si="3"/>
         <v>93</v>
       </c>
-      <c r="I20" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L20" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A21" s="4">
+    <row r="21" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="25">
         <v>193014005</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="26" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="6">
+      <c r="C21" s="27">
         <v>30</v>
       </c>
-      <c r="D21" s="6">
-        <v>10</v>
-      </c>
-      <c r="E21">
+      <c r="D21" s="27">
+        <v>30</v>
+      </c>
+      <c r="E21" s="27">
+        <v>10</v>
+      </c>
+      <c r="F21" s="27">
+        <v>20</v>
+      </c>
+      <c r="G21" s="28">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F21">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-      <c r="H21" s="10">
-        <f t="shared" si="2"/>
+      <c r="H21" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I21" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J21" s="28">
+        <v>10</v>
+      </c>
+      <c r="K21" s="29">
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="I21" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L21" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
-    <row r="22" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="4">
+    <row r="22" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="25">
         <v>193014007</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="26" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="6">
+      <c r="C22" s="27">
         <v>25</v>
       </c>
-      <c r="D22" s="6">
-        <v>0</v>
-      </c>
-      <c r="E22">
+      <c r="D22" s="27">
+        <v>30</v>
+      </c>
+      <c r="E22" s="27">
+        <v>0</v>
+      </c>
+      <c r="F22" s="27">
+        <v>20</v>
+      </c>
+      <c r="G22" s="28">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="F22">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G22">
-        <v>10</v>
-      </c>
-      <c r="H22" s="12">
-        <f t="shared" si="2"/>
+      <c r="H22" s="28">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I22" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="I22" s="28">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J22" s="28">
+        <v>10</v>
+      </c>
+      <c r="K22" s="31">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="L22" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>D</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A23" s="4">
+    <row r="23" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="25">
         <v>193014009</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="27">
         <v>27</v>
       </c>
-      <c r="D23" s="6">
-        <v>8</v>
-      </c>
-      <c r="E23">
+      <c r="D23" s="27">
+        <v>30</v>
+      </c>
+      <c r="E23" s="27">
+        <v>8</v>
+      </c>
+      <c r="F23" s="27">
+        <v>20</v>
+      </c>
+      <c r="G23" s="28">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="F23">
-        <f t="shared" si="1"/>
+      <c r="H23" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I23" s="28">
+        <f t="shared" si="2"/>
         <v>7</v>
       </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23" s="10">
-        <f t="shared" si="2"/>
+      <c r="J23" s="28">
+        <v>10</v>
+      </c>
+      <c r="K23" s="29">
+        <f t="shared" si="3"/>
         <v>70</v>
       </c>
-      <c r="I23" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L23" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A24" s="4">
+    <row r="24" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="25">
         <v>193014010</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="27">
         <v>21.5</v>
       </c>
-      <c r="D24" s="6">
+      <c r="D24" s="27">
+        <v>30</v>
+      </c>
+      <c r="E24" s="27">
         <v>8.5</v>
       </c>
-      <c r="E24">
+      <c r="F24" s="27">
+        <v>20</v>
+      </c>
+      <c r="G24" s="28">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="F24">
-        <f t="shared" si="1"/>
+      <c r="H24" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I24" s="28">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G24">
-        <v>10</v>
-      </c>
-      <c r="H24" s="12">
-        <f t="shared" si="2"/>
+      <c r="J24" s="28">
+        <v>10</v>
+      </c>
+      <c r="K24" s="31">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="I24" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L24" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A25" s="4">
+    <row r="25" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="25">
         <v>193014015</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="26" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="6">
-        <v>0</v>
-      </c>
-      <c r="D25" s="6">
-        <v>0</v>
-      </c>
-      <c r="E25">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F25">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G25">
-        <v>10</v>
-      </c>
-      <c r="H25" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I25" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C25" s="27">
+        <v>0</v>
+      </c>
+      <c r="D25" s="27">
+        <v>30</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0</v>
+      </c>
+      <c r="F25" s="27">
+        <v>20</v>
+      </c>
+      <c r="G25" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I25" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J25" s="28">
+        <v>10</v>
+      </c>
+      <c r="K25" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L25" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="26" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="4">
+    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="25">
         <v>193014016</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="26" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="6">
-        <v>0</v>
-      </c>
-      <c r="D26" s="6">
-        <v>0</v>
-      </c>
-      <c r="E26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F26">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G26">
-        <v>10</v>
-      </c>
-      <c r="H26" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I26" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C26" s="27">
+        <v>0</v>
+      </c>
+      <c r="D26" s="27">
+        <v>30</v>
+      </c>
+      <c r="E26" s="27">
+        <v>0</v>
+      </c>
+      <c r="F26" s="27">
+        <v>20</v>
+      </c>
+      <c r="G26" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I26" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J26" s="28">
+        <v>10</v>
+      </c>
+      <c r="K26" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L26" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="27" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A27" s="4">
+    <row r="27" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A27" s="25">
         <v>193014019</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="26" t="s">
         <v>31</v>
       </c>
-      <c r="C27" s="6">
+      <c r="C27" s="27">
         <v>30</v>
       </c>
-      <c r="D27" s="6">
-        <v>0</v>
-      </c>
-      <c r="E27">
-        <f t="shared" si="0"/>
+      <c r="D27" s="27">
         <v>30</v>
       </c>
-      <c r="F27">
-        <f t="shared" si="1"/>
+      <c r="E27" s="27">
+        <v>0</v>
+      </c>
+      <c r="F27" s="27">
+        <v>20</v>
+      </c>
+      <c r="G27" s="28">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="H27" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I27" s="28">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="G27">
-        <v>10</v>
-      </c>
-      <c r="H27" s="10">
-        <f t="shared" si="2"/>
+      <c r="J27" s="28">
+        <v>10</v>
+      </c>
+      <c r="K27" s="29">
+        <f t="shared" si="3"/>
         <v>60</v>
       </c>
-      <c r="I27" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L27" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C+</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A28" s="4">
+    <row r="28" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A28" s="25">
         <v>193014026</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="26" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="6">
+      <c r="C28" s="27">
         <v>25</v>
       </c>
-      <c r="D28" s="6">
+      <c r="D28" s="27">
+        <v>30</v>
+      </c>
+      <c r="E28" s="27">
         <v>13</v>
       </c>
-      <c r="E28">
+      <c r="F28" s="27">
+        <v>20</v>
+      </c>
+      <c r="G28" s="28">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F28">
-        <f t="shared" si="1"/>
+      <c r="H28" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I28" s="28">
+        <f t="shared" si="2"/>
         <v>7.6</v>
       </c>
-      <c r="G28">
-        <v>10</v>
-      </c>
-      <c r="H28" s="12">
-        <f t="shared" si="2"/>
+      <c r="J28" s="28">
+        <v>10</v>
+      </c>
+      <c r="K28" s="31">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="I28" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L28" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
-    <row r="29" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A29" s="4">
+    <row r="29" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A29" s="25">
         <v>193014030</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C29" s="6">
+      <c r="C29" s="27">
         <v>23.5</v>
       </c>
-      <c r="D29" s="6">
+      <c r="D29" s="27">
+        <v>30</v>
+      </c>
+      <c r="E29" s="27">
         <v>13</v>
       </c>
-      <c r="E29">
+      <c r="F29" s="27">
+        <v>20</v>
+      </c>
+      <c r="G29" s="28">
         <f t="shared" si="0"/>
         <v>36.5</v>
       </c>
-      <c r="F29">
-        <f t="shared" si="1"/>
+      <c r="H29" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I29" s="28">
+        <f t="shared" si="2"/>
         <v>7.3</v>
       </c>
-      <c r="G29">
-        <v>10</v>
-      </c>
-      <c r="H29" s="12">
-        <f t="shared" si="2"/>
+      <c r="J29" s="28">
+        <v>10</v>
+      </c>
+      <c r="K29" s="31">
+        <f t="shared" si="3"/>
         <v>73</v>
       </c>
-      <c r="I29" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L29" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
-    <row r="30" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A30" s="4">
+    <row r="30" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A30" s="25">
         <v>193014032</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="26" t="s">
         <v>34</v>
       </c>
-      <c r="C30" s="6">
-        <v>0</v>
-      </c>
-      <c r="D30" s="6">
-        <v>0</v>
-      </c>
-      <c r="E30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F30">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G30">
-        <v>10</v>
-      </c>
-      <c r="H30" s="10">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="C30" s="27">
+        <v>0</v>
+      </c>
+      <c r="D30" s="27">
+        <v>30</v>
+      </c>
+      <c r="E30" s="27">
+        <v>0</v>
+      </c>
+      <c r="F30" s="27">
+        <v>20</v>
+      </c>
+      <c r="G30" s="28">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I30" s="28">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J30" s="28">
+        <v>10</v>
+      </c>
+      <c r="K30" s="29">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="L30" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
-    <row r="31" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A31" s="4">
+    <row r="31" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A31" s="25">
         <v>193014033</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="26" t="s">
         <v>35</v>
       </c>
-      <c r="C31" s="6">
+      <c r="C31" s="27">
         <v>26.5</v>
       </c>
-      <c r="D31" s="6">
+      <c r="D31" s="27">
+        <v>30</v>
+      </c>
+      <c r="E31" s="27">
         <v>18</v>
       </c>
-      <c r="E31">
+      <c r="F31" s="27">
+        <v>20</v>
+      </c>
+      <c r="G31" s="28">
         <f t="shared" si="0"/>
         <v>44.5</v>
       </c>
-      <c r="F31">
-        <f t="shared" si="1"/>
+      <c r="H31" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I31" s="28">
+        <f t="shared" si="2"/>
         <v>8.9</v>
       </c>
-      <c r="G31">
-        <v>10</v>
-      </c>
-      <c r="H31" s="12">
-        <f t="shared" si="2"/>
+      <c r="J31" s="28">
+        <v>10</v>
+      </c>
+      <c r="K31" s="31">
+        <f t="shared" si="3"/>
         <v>89</v>
       </c>
-      <c r="I31" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L31" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
-    <row r="32" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A32" s="4">
+    <row r="32" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A32" s="25">
         <v>193014035</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="C32" s="6">
+      <c r="C32" s="27">
         <v>7</v>
       </c>
-      <c r="D32" s="6">
+      <c r="D32" s="27">
+        <v>30</v>
+      </c>
+      <c r="E32" s="27">
         <v>18</v>
       </c>
-      <c r="E32">
+      <c r="F32" s="27">
+        <v>20</v>
+      </c>
+      <c r="G32" s="28">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="F32">
-        <f t="shared" si="1"/>
-        <v>5</v>
-      </c>
-      <c r="G32">
-        <v>10</v>
-      </c>
-      <c r="H32" s="12">
-        <f t="shared" si="2"/>
+      <c r="H32" s="28">
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
-      <c r="I32" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="I32" s="28">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="J32" s="28">
+        <v>10</v>
+      </c>
+      <c r="K32" s="31">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+      <c r="L32" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>D</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A33" s="4">
+    <row r="33" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A33" s="25">
         <v>193014036</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="26" t="s">
         <v>37</v>
       </c>
-      <c r="C33" s="6">
+      <c r="C33" s="27">
         <v>22</v>
       </c>
-      <c r="D33" s="6">
+      <c r="D33" s="27">
+        <v>30</v>
+      </c>
+      <c r="E33" s="27">
         <v>11</v>
       </c>
-      <c r="E33">
+      <c r="F33" s="27">
+        <v>20</v>
+      </c>
+      <c r="G33" s="28">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="F33">
-        <f t="shared" si="1"/>
-        <v>6.6</v>
-      </c>
-      <c r="G33">
-        <v>10</v>
-      </c>
-      <c r="H33" s="12">
-        <f t="shared" si="2"/>
-        <v>65.999999999999986</v>
-      </c>
-      <c r="I33" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="H33" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I33" s="28">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="J33" s="28">
+        <v>10</v>
+      </c>
+      <c r="K33" s="31">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="L33" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
-    <row r="34" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A34" s="4">
+    <row r="34" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A34" s="25">
         <v>193014040</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="26" t="s">
         <v>38</v>
       </c>
-      <c r="C34" s="6">
+      <c r="C34" s="27">
         <v>30</v>
       </c>
-      <c r="D34" s="6">
+      <c r="D34" s="27">
+        <v>30</v>
+      </c>
+      <c r="E34" s="27">
         <v>11</v>
       </c>
-      <c r="E34">
+      <c r="F34" s="27">
+        <v>20</v>
+      </c>
+      <c r="G34" s="28">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="F34">
-        <f t="shared" si="1"/>
+      <c r="H34" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I34" s="28">
+        <f t="shared" si="2"/>
         <v>8.1999999999999993</v>
       </c>
-      <c r="G34">
-        <v>10</v>
-      </c>
-      <c r="H34" s="10">
-        <f t="shared" si="2"/>
+      <c r="J34" s="28">
+        <v>10</v>
+      </c>
+      <c r="K34" s="29">
+        <f t="shared" si="3"/>
         <v>82</v>
       </c>
-      <c r="I34" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L34" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
-    <row r="35" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A35" s="4">
+    <row r="35" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A35" s="25">
         <v>193014042</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="C35" s="6">
+      <c r="C35" s="27">
         <v>27</v>
       </c>
-      <c r="D35" s="6">
+      <c r="D35" s="27">
+        <v>30</v>
+      </c>
+      <c r="E35" s="27">
         <v>11</v>
       </c>
-      <c r="E35">
+      <c r="F35" s="27">
+        <v>20</v>
+      </c>
+      <c r="G35" s="28">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="F35">
-        <f t="shared" si="1"/>
+      <c r="H35" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I35" s="28">
+        <f t="shared" si="2"/>
         <v>7.6</v>
       </c>
-      <c r="G35">
-        <v>10</v>
-      </c>
-      <c r="H35" s="10">
-        <f t="shared" si="2"/>
+      <c r="J35" s="28">
+        <v>10</v>
+      </c>
+      <c r="K35" s="29">
+        <f t="shared" si="3"/>
         <v>76</v>
       </c>
-      <c r="I35" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L35" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B+</v>
       </c>
     </row>
-    <row r="36" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A36" s="4">
+    <row r="36" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A36" s="25">
         <v>193014048</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C36" s="6">
+      <c r="C36" s="27">
         <v>15</v>
       </c>
-      <c r="D36" s="6">
+      <c r="D36" s="27">
+        <v>30</v>
+      </c>
+      <c r="E36" s="27">
         <v>18</v>
       </c>
-      <c r="E36">
+      <c r="F36" s="27">
+        <v>20</v>
+      </c>
+      <c r="G36" s="28">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="F36">
-        <f t="shared" si="1"/>
-        <v>6.6</v>
-      </c>
-      <c r="G36">
-        <v>10</v>
-      </c>
-      <c r="H36" s="10">
-        <f t="shared" si="2"/>
-        <v>65.999999999999986</v>
-      </c>
-      <c r="I36" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="H36" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I36" s="28">
+        <f t="shared" si="2"/>
+        <v>6.6000000000000005</v>
+      </c>
+      <c r="J36" s="28">
+        <v>10</v>
+      </c>
+      <c r="K36" s="29">
+        <f t="shared" si="3"/>
+        <v>66</v>
+      </c>
+      <c r="L36" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
-    <row r="37" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A37" s="4">
+    <row r="37" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A37" s="25">
         <v>193014050</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="26" t="s">
         <v>41</v>
       </c>
-      <c r="C37" s="6">
+      <c r="C37" s="27">
         <v>30</v>
       </c>
-      <c r="D37" s="6">
+      <c r="D37" s="27">
+        <v>30</v>
+      </c>
+      <c r="E37" s="27">
         <v>18.5</v>
       </c>
-      <c r="E37">
+      <c r="F37" s="27">
+        <v>20</v>
+      </c>
+      <c r="G37" s="28">
         <f t="shared" si="0"/>
         <v>48.5</v>
       </c>
-      <c r="F37">
-        <f t="shared" si="1"/>
+      <c r="H37" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I37" s="28">
+        <f t="shared" si="2"/>
         <v>9.6999999999999993</v>
       </c>
-      <c r="G37">
-        <v>10</v>
-      </c>
-      <c r="H37" s="10">
-        <f t="shared" si="2"/>
+      <c r="J37" s="28">
+        <v>10</v>
+      </c>
+      <c r="K37" s="29">
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
-      <c r="I37" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L37" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A38" s="4">
+    <row r="38" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A38" s="25">
         <v>193014052</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C38" s="6">
+      <c r="C38" s="27">
         <v>30</v>
       </c>
-      <c r="D38" s="6">
+      <c r="D38" s="27">
+        <v>30</v>
+      </c>
+      <c r="E38" s="27">
         <v>18</v>
       </c>
-      <c r="E38">
+      <c r="F38" s="27">
+        <v>20</v>
+      </c>
+      <c r="G38" s="28">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="F38">
-        <f t="shared" si="1"/>
+      <c r="H38" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I38" s="28">
+        <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
-      <c r="G38">
-        <v>10</v>
-      </c>
-      <c r="H38" s="10">
-        <f t="shared" si="2"/>
+      <c r="J38" s="28">
+        <v>10</v>
+      </c>
+      <c r="K38" s="29">
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="I38" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L38" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A39" s="4">
+    <row r="39" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A39" s="25">
         <v>193014053</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="26" t="s">
         <v>43</v>
       </c>
-      <c r="C39" s="6">
+      <c r="C39" s="27">
         <v>28</v>
       </c>
-      <c r="D39" s="6">
-        <v>0</v>
-      </c>
-      <c r="E39">
+      <c r="D39" s="27">
+        <v>30</v>
+      </c>
+      <c r="E39" s="27">
+        <v>0</v>
+      </c>
+      <c r="F39" s="27">
+        <v>20</v>
+      </c>
+      <c r="G39" s="28">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="F39">
-        <f t="shared" si="1"/>
-        <v>5.6</v>
-      </c>
-      <c r="G39">
-        <v>10</v>
-      </c>
-      <c r="H39" s="12">
-        <f t="shared" si="2"/>
-        <v>55.999999999999993</v>
-      </c>
-      <c r="I39" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="H39" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I39" s="28">
+        <f t="shared" si="2"/>
+        <v>5.6000000000000005</v>
+      </c>
+      <c r="J39" s="28">
+        <v>10</v>
+      </c>
+      <c r="K39" s="31">
+        <f t="shared" si="3"/>
+        <v>56.000000000000007</v>
+      </c>
+      <c r="L39" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
-    <row r="40" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A40" s="4">
+    <row r="40" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A40" s="25">
         <v>193014055</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="26" t="s">
         <v>44</v>
       </c>
-      <c r="C40" s="6">
+      <c r="C40" s="27">
         <v>16</v>
       </c>
-      <c r="D40" s="6">
+      <c r="D40" s="27">
+        <v>30</v>
+      </c>
+      <c r="E40" s="27">
         <v>18</v>
       </c>
-      <c r="E40">
+      <c r="F40" s="27">
+        <v>20</v>
+      </c>
+      <c r="G40" s="28">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="F40">
-        <f t="shared" si="1"/>
-        <v>6.8</v>
-      </c>
-      <c r="G40">
-        <v>10</v>
-      </c>
-      <c r="H40" s="12">
-        <f t="shared" si="2"/>
+      <c r="H40" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I40" s="28">
+        <f t="shared" si="2"/>
+        <v>6.8000000000000007</v>
+      </c>
+      <c r="J40" s="28">
+        <v>10</v>
+      </c>
+      <c r="K40" s="31">
+        <f t="shared" si="3"/>
         <v>68</v>
       </c>
-      <c r="I40" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L40" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B-</v>
       </c>
     </row>
-    <row r="41" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A41" s="4">
+    <row r="41" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A41" s="25">
         <v>193014056</v>
       </c>
-      <c r="B41" s="3" t="s">
+      <c r="B41" s="26" t="s">
         <v>45</v>
       </c>
-      <c r="C41" s="6">
+      <c r="C41" s="27">
         <v>30</v>
       </c>
-      <c r="D41" s="6">
+      <c r="D41" s="27">
+        <v>30</v>
+      </c>
+      <c r="E41" s="27">
         <v>18</v>
       </c>
-      <c r="E41">
+      <c r="F41" s="27">
+        <v>20</v>
+      </c>
+      <c r="G41" s="28">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="F41">
-        <f t="shared" si="1"/>
+      <c r="H41" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I41" s="28">
+        <f t="shared" si="2"/>
         <v>9.6</v>
       </c>
-      <c r="G41">
-        <v>10</v>
-      </c>
-      <c r="H41" s="10">
-        <f t="shared" si="2"/>
+      <c r="J41" s="28">
+        <v>10</v>
+      </c>
+      <c r="K41" s="29">
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
-      <c r="I41" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L41" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A+</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A42" s="4">
+    <row r="42" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="25">
         <v>193014060</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="6">
+      <c r="C42" s="27">
         <v>25</v>
       </c>
-      <c r="D42" s="6">
+      <c r="D42" s="27">
+        <v>30</v>
+      </c>
+      <c r="E42" s="27">
         <v>15</v>
       </c>
-      <c r="E42">
+      <c r="F42" s="27">
+        <v>20</v>
+      </c>
+      <c r="G42" s="28">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="F42">
-        <f t="shared" si="1"/>
-        <v>8</v>
-      </c>
-      <c r="G42">
-        <v>10</v>
-      </c>
-      <c r="H42" s="12">
-        <f t="shared" si="2"/>
+      <c r="H42" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I42" s="28">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="J42" s="28">
+        <v>10</v>
+      </c>
+      <c r="K42" s="31">
+        <f t="shared" si="3"/>
         <v>80</v>
       </c>
-      <c r="I42" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L42" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A-</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A43" s="4">
+    <row r="43" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="25">
         <v>193014061</v>
       </c>
-      <c r="B43" s="3" t="s">
+      <c r="B43" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="6">
+      <c r="C43" s="27">
         <v>25</v>
       </c>
-      <c r="D43" s="6">
+      <c r="D43" s="27">
+        <v>30</v>
+      </c>
+      <c r="E43" s="27">
         <v>18</v>
       </c>
-      <c r="E43">
+      <c r="F43" s="27">
+        <v>20</v>
+      </c>
+      <c r="G43" s="28">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="F43">
-        <f t="shared" si="1"/>
+      <c r="H43" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I43" s="28">
+        <f t="shared" si="2"/>
         <v>8.6</v>
       </c>
-      <c r="G43">
-        <v>10</v>
-      </c>
-      <c r="H43" s="12">
-        <f t="shared" si="2"/>
+      <c r="J43" s="28">
+        <v>10</v>
+      </c>
+      <c r="K43" s="31">
+        <f t="shared" si="3"/>
         <v>86</v>
       </c>
-      <c r="I43" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L43" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
-    <row r="44" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A44" s="4">
+    <row r="44" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="25">
         <v>193014062</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="26" t="s">
         <v>48</v>
       </c>
-      <c r="C44" s="6">
+      <c r="C44" s="27">
         <v>29</v>
       </c>
-      <c r="D44" s="6">
-        <v>0</v>
-      </c>
-      <c r="E44">
+      <c r="D44" s="27">
+        <v>30</v>
+      </c>
+      <c r="E44" s="27">
+        <v>0</v>
+      </c>
+      <c r="F44" s="27">
+        <v>20</v>
+      </c>
+      <c r="G44" s="28">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="F44">
-        <f t="shared" si="1"/>
+      <c r="H44" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I44" s="28">
+        <f t="shared" si="2"/>
         <v>5.8</v>
       </c>
-      <c r="G44">
-        <v>10</v>
-      </c>
-      <c r="H44" s="12">
-        <f t="shared" si="2"/>
+      <c r="J44" s="28">
+        <v>10</v>
+      </c>
+      <c r="K44" s="31">
+        <f t="shared" si="3"/>
         <v>57.999999999999993</v>
       </c>
-      <c r="I44" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L44" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
-    <row r="45" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A45" s="4">
+    <row r="45" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A45" s="25">
         <v>193014064</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="26" t="s">
         <v>49</v>
       </c>
-      <c r="C45" s="6">
+      <c r="C45" s="27">
         <v>29</v>
       </c>
-      <c r="D45" s="6">
-        <v>0</v>
-      </c>
-      <c r="E45">
+      <c r="D45" s="27">
+        <v>30</v>
+      </c>
+      <c r="E45" s="27">
+        <v>0</v>
+      </c>
+      <c r="F45" s="27">
+        <v>20</v>
+      </c>
+      <c r="G45" s="28">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="F45">
-        <f t="shared" si="1"/>
+      <c r="H45" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I45" s="28">
+        <f t="shared" si="2"/>
         <v>5.8</v>
       </c>
-      <c r="G45">
-        <v>10</v>
-      </c>
-      <c r="H45" s="12">
-        <f t="shared" si="2"/>
+      <c r="J45" s="28">
+        <v>10</v>
+      </c>
+      <c r="K45" s="31">
+        <f t="shared" si="3"/>
         <v>57.999999999999993</v>
       </c>
-      <c r="I45" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L45" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>C</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A46" s="4">
+    <row r="46" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A46" s="25">
         <v>193014065</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="26" t="s">
         <v>50</v>
       </c>
-      <c r="C46" s="6">
+      <c r="C46" s="27">
         <v>25</v>
       </c>
-      <c r="D46" s="6">
+      <c r="D46" s="27">
+        <v>30</v>
+      </c>
+      <c r="E46" s="27">
         <v>17.5</v>
       </c>
-      <c r="E46">
+      <c r="F46" s="27">
+        <v>20</v>
+      </c>
+      <c r="G46" s="28">
         <f t="shared" si="0"/>
         <v>42.5</v>
       </c>
-      <c r="F46">
-        <f t="shared" si="1"/>
+      <c r="H46" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I46" s="28">
+        <f t="shared" si="2"/>
         <v>8.5</v>
       </c>
-      <c r="G46">
-        <v>10</v>
-      </c>
-      <c r="H46" s="12">
-        <f t="shared" si="2"/>
+      <c r="J46" s="28">
+        <v>10</v>
+      </c>
+      <c r="K46" s="31">
+        <f t="shared" si="3"/>
         <v>85</v>
       </c>
-      <c r="I46" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L46" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>A</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A47" s="4">
+    <row r="47" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A47" s="25">
         <v>193014067</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="26" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="6">
+      <c r="C47" s="27">
         <v>27</v>
       </c>
-      <c r="D47" s="6">
+      <c r="D47" s="27">
+        <v>30</v>
+      </c>
+      <c r="E47" s="27">
         <v>9</v>
       </c>
-      <c r="E47">
+      <c r="F47" s="27">
+        <v>20</v>
+      </c>
+      <c r="G47" s="28">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="F47">
-        <f t="shared" si="1"/>
-        <v>7.2</v>
-      </c>
-      <c r="G47">
-        <v>10</v>
-      </c>
-      <c r="H47" s="10">
-        <f t="shared" si="2"/>
+      <c r="H47" s="28">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I47" s="28">
+        <f t="shared" si="2"/>
+        <v>7.1999999999999993</v>
+      </c>
+      <c r="J47" s="28">
+        <v>10</v>
+      </c>
+      <c r="K47" s="29">
+        <f t="shared" si="3"/>
         <v>72</v>
       </c>
-      <c r="I47" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L47" s="30" t="str">
+        <f t="shared" si="4"/>
         <v>B</v>
       </c>
     </row>
-    <row r="48" spans="1:9" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:12" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="32">
         <v>193014069</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="6">
+      <c r="C48" s="16">
         <v>4</v>
       </c>
-      <c r="D48" s="6">
+      <c r="D48" s="16">
+        <v>30</v>
+      </c>
+      <c r="E48" s="16">
         <v>17.5</v>
       </c>
-      <c r="E48">
+      <c r="F48" s="16">
+        <v>20</v>
+      </c>
+      <c r="G48" s="20">
         <f t="shared" si="0"/>
         <v>21.5</v>
       </c>
-      <c r="F48">
-        <f t="shared" si="1"/>
+      <c r="H48" s="20">
+        <f t="shared" si="1"/>
+        <v>50</v>
+      </c>
+      <c r="I48" s="20">
+        <f t="shared" si="2"/>
         <v>4.3</v>
       </c>
-      <c r="G48">
-        <v>10</v>
-      </c>
-      <c r="H48" s="12">
-        <f t="shared" si="2"/>
+      <c r="J48" s="20">
+        <v>10</v>
+      </c>
+      <c r="K48" s="17">
+        <f t="shared" si="3"/>
         <v>43</v>
       </c>
-      <c r="I48" s="11" t="str">
-        <f t="shared" si="3"/>
+      <c r="L48" s="33" t="str">
+        <f t="shared" si="4"/>
         <v>F</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9769,8 +10381,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:N48"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:N48"/>
+    <sheetView topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D51" sqref="D51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11897,48 +12509,48 @@
         <v>F</v>
       </c>
     </row>
-    <row r="48" spans="1:14" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:14" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="13">
         <v>193014069</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C48" s="15">
         <v>2</v>
       </c>
-      <c r="D48" s="5">
-        <v>5</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5">
+      <c r="D48" s="15">
+        <v>5</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15">
         <v>6</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G48" s="15">
         <v>2</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H48" s="15">
         <v>3</v>
       </c>
-      <c r="I48" s="5">
+      <c r="I48" s="15">
         <v>1</v>
       </c>
-      <c r="J48" s="5">
+      <c r="J48" s="15">
         <v>6</v>
       </c>
-      <c r="K48" s="6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="L48" s="6">
+      <c r="K48" s="16">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="L48" s="16">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="M48" s="10">
+      <c r="M48" s="21">
         <f t="shared" si="2"/>
         <v>25</v>
       </c>
-      <c r="N48" s="11" t="str">
+      <c r="N48" s="18" t="str">
         <f t="shared" si="3"/>
         <v>F</v>
       </c>
@@ -11973,8 +12585,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{485E7955-23DA-41EB-BFE8-1A0365DA72E9}">
   <dimension ref="A1:P48"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12016,10 +12628,10 @@
         <v>59</v>
       </c>
       <c r="K1" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>65</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>66</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>60</v>
@@ -12106,19 +12718,19 @@
         <v>10</v>
       </c>
       <c r="M3" s="6">
-        <f>C3+E3+G3+I3</f>
+        <f t="shared" ref="M3:M48" si="0">C3+E3+G3+I3</f>
         <v>0</v>
       </c>
       <c r="N3" s="6">
-        <f t="shared" ref="N3:N48" si="0">D3+F3+H3+J3+L3</f>
+        <f t="shared" ref="N3:N48" si="1">D3+F3+H3+J3+L3</f>
         <v>40</v>
       </c>
       <c r="O3" s="10">
-        <f t="shared" ref="O3:O48" si="1">(M3/N3)*100</f>
+        <f t="shared" ref="O3:O48" si="2">(M3/N3)*100</f>
         <v>0</v>
       </c>
       <c r="P3" s="11" t="str">
-        <f t="shared" ref="P3:P48" si="2">IF(O3&gt;94,"A+",IF(O3&gt;84,"A",IF(O3&gt;79,"A-",IF(O3&gt;74,"B+",IF(O3&gt;69,"B",IF(O3&gt;64,"B-",IF(O3&gt;59,"C+",IF(O3&gt;54,"C",IF(O3&gt;49,"D","F")))))))))</f>
+        <f t="shared" ref="P3:P48" si="3">IF(O3&gt;94,"A+",IF(O3&gt;84,"A",IF(O3&gt;79,"A-",IF(O3&gt;74,"B+",IF(O3&gt;69,"B",IF(O3&gt;64,"B-",IF(O3&gt;59,"C+",IF(O3&gt;54,"C",IF(O3&gt;49,"D","F")))))))))</f>
         <v>F</v>
       </c>
     </row>
@@ -12150,19 +12762,19 @@
         <v>10</v>
       </c>
       <c r="M4" s="6">
-        <f>C4+E4+G4+I4</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N4" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O4" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P4" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12194,19 +12806,19 @@
         <v>10</v>
       </c>
       <c r="M5" s="6">
-        <f>C5+E5+G5+I5</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N5" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O5" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P5" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12238,19 +12850,19 @@
         <v>10</v>
       </c>
       <c r="M6" s="6">
-        <f>C6+E6+G6+I6</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N6" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O6" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P6" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12282,19 +12894,19 @@
         <v>10</v>
       </c>
       <c r="M7" s="6">
-        <f>C7+E7+G7+I7</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N7" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O7" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P7" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12326,19 +12938,19 @@
         <v>10</v>
       </c>
       <c r="M8" s="6">
-        <f>C8+E8+G8+I8</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N8" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O8" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P8" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12370,19 +12982,19 @@
         <v>10</v>
       </c>
       <c r="M9" s="6">
-        <f>C9+E9+G9+I9</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N9" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O9" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P9" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12414,19 +13026,19 @@
         <v>10</v>
       </c>
       <c r="M10" s="6">
-        <f>C10+E10+G10+I10</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N10" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O10" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P10" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12458,19 +13070,19 @@
         <v>10</v>
       </c>
       <c r="M11" s="6">
-        <f>C11+E11+G11+I11</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N11" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O11" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P11" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12498,19 +13110,19 @@
         <v>10</v>
       </c>
       <c r="M12" s="6">
-        <f>C12+E12+G12+I12</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N12" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O12" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P12" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12542,19 +13154,19 @@
         <v>10</v>
       </c>
       <c r="M13" s="6">
-        <f>C13+E13+G13+I13</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N13" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P13" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12586,19 +13198,19 @@
         <v>10</v>
       </c>
       <c r="M14" s="6">
-        <f>C14+E14+G14+I14</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N14" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P14" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12630,19 +13242,19 @@
         <v>10</v>
       </c>
       <c r="M15" s="6">
-        <f>C15+E15+G15+I15</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N15" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O15" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P15" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12674,19 +13286,19 @@
         <v>10</v>
       </c>
       <c r="M16" s="6">
-        <f>C16+E16+G16+I16</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N16" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P16" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12718,19 +13330,19 @@
         <v>10</v>
       </c>
       <c r="M17" s="6">
-        <f>C17+E17+G17+I17</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N17" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O17" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P17" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12762,19 +13374,19 @@
         <v>10</v>
       </c>
       <c r="M18" s="6">
-        <f>C18+E18+G18+I18</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N18" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P18" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12806,19 +13418,19 @@
         <v>10</v>
       </c>
       <c r="M19" s="6">
-        <f>C19+E19+G19+I19</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N19" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P19" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12850,19 +13462,19 @@
         <v>10</v>
       </c>
       <c r="M20" s="6">
-        <f>C20+E20+G20+I20</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N20" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P20" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12894,19 +13506,19 @@
         <v>10</v>
       </c>
       <c r="M21" s="6">
-        <f>C21+E21+G21+I21</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N21" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O21" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P21" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12938,19 +13550,19 @@
         <v>10</v>
       </c>
       <c r="M22" s="6">
-        <f>C22+E22+G22+I22</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N22" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O22" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P22" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -12982,19 +13594,19 @@
         <v>10</v>
       </c>
       <c r="M23" s="6">
-        <f>C23+E23+G23+I23</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N23" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O23" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P23" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13026,19 +13638,19 @@
         <v>10</v>
       </c>
       <c r="M24" s="6">
-        <f>C24+E24+G24+I24</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N24" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O24" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P24" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13070,19 +13682,19 @@
         <v>10</v>
       </c>
       <c r="M25" s="6">
-        <f>C25+E25+G25+I25</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N25" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O25" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P25" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13114,19 +13726,19 @@
         <v>10</v>
       </c>
       <c r="M26" s="6">
-        <f>C26+E26+G26+I26</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N26" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O26" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P26" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13158,19 +13770,19 @@
         <v>10</v>
       </c>
       <c r="M27" s="6">
-        <f>C27+E27+G27+I27</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N27" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O27" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P27" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13202,19 +13814,19 @@
         <v>10</v>
       </c>
       <c r="M28" s="6">
-        <f>C28+E28+G28+I28</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N28" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O28" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P28" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13246,19 +13858,19 @@
         <v>10</v>
       </c>
       <c r="M29" s="6">
-        <f>C29+E29+G29+I29</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N29" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O29" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P29" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13290,19 +13902,19 @@
         <v>10</v>
       </c>
       <c r="M30" s="6">
-        <f>C30+E30+G30+I30</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N30" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O30" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P30" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13334,19 +13946,19 @@
         <v>10</v>
       </c>
       <c r="M31" s="6">
-        <f>C31+E31+G31+I31</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N31" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O31" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P31" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13378,19 +13990,19 @@
         <v>10</v>
       </c>
       <c r="M32" s="6">
-        <f>C32+E32+G32+I32</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N32" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O32" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P32" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13422,19 +14034,19 @@
         <v>10</v>
       </c>
       <c r="M33" s="6">
-        <f>C33+E33+G33+I33</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N33" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O33" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P33" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13466,19 +14078,19 @@
         <v>10</v>
       </c>
       <c r="M34" s="6">
-        <f>C34+E34+G34+I34</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N34" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O34" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P34" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13510,19 +14122,19 @@
         <v>10</v>
       </c>
       <c r="M35" s="6">
-        <f>C35+E35+G35+I35</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N35" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O35" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P35" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13554,19 +14166,19 @@
         <v>10</v>
       </c>
       <c r="M36" s="6">
-        <f>C36+E36+G36+I36</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N36" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O36" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P36" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13598,19 +14210,19 @@
         <v>10</v>
       </c>
       <c r="M37" s="6">
-        <f>C37+E37+G37+I37</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N37" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O37" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P37" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13642,19 +14254,19 @@
         <v>10</v>
       </c>
       <c r="M38" s="6">
-        <f>C38+E38+G38+I38</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N38" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O38" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P38" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13686,19 +14298,19 @@
         <v>10</v>
       </c>
       <c r="M39" s="6">
-        <f>C39+E39+G39+I39</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N39" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O39" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P39" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13730,19 +14342,19 @@
         <v>10</v>
       </c>
       <c r="M40" s="6">
-        <f>C40+E40+G40+I40</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N40" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O40" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P40" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13774,19 +14386,19 @@
         <v>10</v>
       </c>
       <c r="M41" s="6">
-        <f>C41+E41+G41+I41</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N41" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O41" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P41" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13818,19 +14430,19 @@
         <v>10</v>
       </c>
       <c r="M42" s="6">
-        <f>C42+E42+G42+I42</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N42" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O42" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P42" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13862,19 +14474,19 @@
         <v>10</v>
       </c>
       <c r="M43" s="6">
-        <f>C43+E43+G43+I43</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N43" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O43" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P43" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13906,19 +14518,19 @@
         <v>10</v>
       </c>
       <c r="M44" s="6">
-        <f>C44+E44+G44+I44</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N44" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O44" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P44" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13950,19 +14562,19 @@
         <v>10</v>
       </c>
       <c r="M45" s="6">
-        <f>C45+E45+G45+I45</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N45" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O45" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P45" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -13994,19 +14606,19 @@
         <v>10</v>
       </c>
       <c r="M46" s="6">
-        <f>C46+E46+G46+I46</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N46" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O46" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P46" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
@@ -14038,63 +14650,63 @@
         <v>10</v>
       </c>
       <c r="M47" s="6">
-        <f>C47+E47+G47+I47</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="N47" s="6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="O47" s="10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="P47" s="11" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>
-    <row r="48" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A48" s="4">
+    <row r="48" spans="1:16" s="20" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="13">
         <v>193014069</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="5">
-        <v>5</v>
-      </c>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5">
-        <v>5</v>
-      </c>
-      <c r="G48" s="5"/>
-      <c r="H48" s="5">
-        <v>10</v>
-      </c>
-      <c r="I48" s="5"/>
-      <c r="J48" s="5">
-        <v>10</v>
-      </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="5">
-        <v>10</v>
-      </c>
-      <c r="M48" s="6">
-        <f>C48+E48+G48+I48</f>
-        <v>0</v>
-      </c>
-      <c r="N48" s="6">
-        <f t="shared" si="0"/>
+      <c r="C48" s="15"/>
+      <c r="D48" s="15">
+        <v>5</v>
+      </c>
+      <c r="E48" s="15"/>
+      <c r="F48" s="15">
+        <v>5</v>
+      </c>
+      <c r="G48" s="15"/>
+      <c r="H48" s="15">
+        <v>10</v>
+      </c>
+      <c r="I48" s="15"/>
+      <c r="J48" s="15">
+        <v>10</v>
+      </c>
+      <c r="K48" s="15"/>
+      <c r="L48" s="15">
+        <v>10</v>
+      </c>
+      <c r="M48" s="16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N48" s="16">
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
-      <c r="O48" s="10">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="P48" s="11" t="str">
-        <f t="shared" si="2"/>
+      <c r="O48" s="21">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P48" s="18" t="str">
+        <f t="shared" si="3"/>
         <v>F</v>
       </c>
     </row>

</xml_diff>

<commit_message>
added attendance for cse 101 section 9
</commit_message>
<xml_diff>
--- a/FALL 19/CSE 101/results_cse101_sec9.xlsx
+++ b/FALL 19/CSE 101/results_cse101_sec9.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="21840" windowHeight="12570" activeTab="4"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="21840" windowHeight="12570"/>
   </bookViews>
   <sheets>
-    <sheet name="quiz1" sheetId="1" r:id="rId1"/>
-    <sheet name="quiz2" sheetId="3" r:id="rId2"/>
-    <sheet name="quiz_final" sheetId="4" r:id="rId3"/>
-    <sheet name="mid" sheetId="2" r:id="rId4"/>
-    <sheet name="final" sheetId="5" r:id="rId5"/>
-    <sheet name="project" sheetId="6" r:id="rId6"/>
+    <sheet name="attendance" sheetId="7" r:id="rId1"/>
+    <sheet name="quiz1" sheetId="1" r:id="rId2"/>
+    <sheet name="quiz2" sheetId="3" r:id="rId3"/>
+    <sheet name="quiz_final" sheetId="4" r:id="rId4"/>
+    <sheet name="mid" sheetId="2" r:id="rId5"/>
+    <sheet name="final" sheetId="5" r:id="rId6"/>
+    <sheet name="project" sheetId="6" r:id="rId7"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <calcPr calcId="124519"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="73">
   <si>
     <t>ID</t>
   </si>
@@ -244,6 +245,12 @@
   <si>
     <t>Presentation</t>
   </si>
+  <si>
+    <t>Absent</t>
+  </si>
+  <si>
+    <t>Present</t>
+  </si>
 </sst>
 </file>
 
@@ -412,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -512,12 +519,107 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <condense val="0"/>
+        <extend val="0"/>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <condense val="0"/>
@@ -1545,12 +1647,1483 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H49"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" customWidth="1"/>
+    <col min="2" max="2" width="30.7109375" customWidth="1"/>
+    <col min="3" max="8" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" ht="15">
+      <c r="A1" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" s="23" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" s="23" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="23" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" s="24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="15">
+      <c r="A2" s="25">
+        <v>173011011</v>
+      </c>
+      <c r="B2" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="47">
+        <v>21</v>
+      </c>
+      <c r="D2" s="47">
+        <v>15</v>
+      </c>
+      <c r="E2" s="47">
+        <f>C2-D2</f>
+        <v>6</v>
+      </c>
+      <c r="F2" s="27">
+        <f>ROUNDUP((E2/C2)*F$49,0)</f>
+        <v>3</v>
+      </c>
+      <c r="G2" s="29">
+        <f>(F2/F$49)*100</f>
+        <v>30</v>
+      </c>
+      <c r="H2" s="30" t="str">
+        <f>IF(G2&gt;94,"A+",IF(G2&gt;84,"A",IF(G2&gt;79,"A-",IF(G2&gt;74,"B+",IF(G2&gt;69,"B",IF(G2&gt;64,"B-",IF(G2&gt;59,"C+",IF(G2&gt;54,"C",IF(G2&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15">
+      <c r="A3" s="25">
+        <v>181014084</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="48">
+        <v>21</v>
+      </c>
+      <c r="D3" s="48">
+        <v>21</v>
+      </c>
+      <c r="E3" s="47">
+        <f t="shared" ref="E3:E48" si="0">C3-D3</f>
+        <v>0</v>
+      </c>
+      <c r="F3" s="27">
+        <f t="shared" ref="F3:F48" si="1">ROUNDUP((E3/C3)*F$49,0)</f>
+        <v>0</v>
+      </c>
+      <c r="G3" s="29">
+        <f t="shared" ref="G3:G48" si="2">(F3/F$49)*100</f>
+        <v>0</v>
+      </c>
+      <c r="H3" s="30" t="str">
+        <f t="shared" ref="H3:H48" si="3">IF(G3&gt;94,"A+",IF(G3&gt;84,"A",IF(G3&gt;79,"A-",IF(G3&gt;74,"B+",IF(G3&gt;69,"B",IF(G3&gt;64,"B-",IF(G3&gt;59,"C+",IF(G3&gt;54,"C",IF(G3&gt;49,"D","F")))))))))</f>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15">
+      <c r="A4" s="25">
+        <v>183011124</v>
+      </c>
+      <c r="B4" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="47">
+        <v>16</v>
+      </c>
+      <c r="D4" s="47">
+        <v>7</v>
+      </c>
+      <c r="E4" s="47">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="F4" s="27">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G4" s="29">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H4" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15">
+      <c r="A5" s="25">
+        <v>183013056</v>
+      </c>
+      <c r="B5" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="47">
+        <v>21</v>
+      </c>
+      <c r="D5" s="47">
+        <v>10</v>
+      </c>
+      <c r="E5" s="47">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="F5" s="27">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="G5" s="29">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="H5" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>C+</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15">
+      <c r="A6" s="25">
+        <v>183013064</v>
+      </c>
+      <c r="B6" s="26" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="48">
+        <v>16</v>
+      </c>
+      <c r="D6" s="48">
+        <v>14</v>
+      </c>
+      <c r="E6" s="47">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="F6" s="27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G6" s="29">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H6" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15">
+      <c r="A7" s="25">
+        <v>183014013</v>
+      </c>
+      <c r="B7" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="47">
+        <v>21</v>
+      </c>
+      <c r="D7" s="47">
+        <v>6</v>
+      </c>
+      <c r="E7" s="47">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F7" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G7" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H7" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15">
+      <c r="A8" s="25">
+        <v>183014047</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="47">
+        <v>21</v>
+      </c>
+      <c r="D8" s="47">
+        <v>2</v>
+      </c>
+      <c r="E8" s="47">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F8" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G8" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H8" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15">
+      <c r="A9" s="25">
+        <v>183014061</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="48">
+        <v>21</v>
+      </c>
+      <c r="D9" s="48">
+        <v>20</v>
+      </c>
+      <c r="E9" s="47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F9" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G9" s="29">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H9" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15">
+      <c r="A10" s="25">
+        <v>191011024</v>
+      </c>
+      <c r="B10" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="47">
+        <v>21</v>
+      </c>
+      <c r="D10" s="47">
+        <v>5</v>
+      </c>
+      <c r="E10" s="47">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F10" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G10" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H10" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15">
+      <c r="A11" s="25">
+        <v>191014023</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11" s="47">
+        <v>21</v>
+      </c>
+      <c r="D11" s="47">
+        <v>3</v>
+      </c>
+      <c r="E11" s="47">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F11" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G11" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H11" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15">
+      <c r="A12" s="25">
+        <v>191014032</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="49">
+        <v>16</v>
+      </c>
+      <c r="D12" s="49">
+        <v>16</v>
+      </c>
+      <c r="E12" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F12" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15">
+      <c r="A13" s="25">
+        <v>191014069</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="48">
+        <v>16</v>
+      </c>
+      <c r="D13" s="48">
+        <v>4</v>
+      </c>
+      <c r="E13" s="47">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="F13" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G13" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H13" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15">
+      <c r="A14" s="25">
+        <v>192011115</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="47">
+        <v>21</v>
+      </c>
+      <c r="D14" s="47">
+        <v>13</v>
+      </c>
+      <c r="E14" s="47">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="F14" s="27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G14" s="29">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H14" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15">
+      <c r="A15" s="25">
+        <v>192014019</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="47">
+        <v>16</v>
+      </c>
+      <c r="D15" s="47">
+        <v>2</v>
+      </c>
+      <c r="E15" s="47">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F15" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G15" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H15" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="15">
+      <c r="A16" s="25">
+        <v>192014023</v>
+      </c>
+      <c r="B16" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="48">
+        <v>16</v>
+      </c>
+      <c r="D16" s="48">
+        <v>15</v>
+      </c>
+      <c r="E16" s="47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="F16" s="27">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="G16" s="29">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="H16" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="15">
+      <c r="A17" s="25">
+        <v>192014029</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" s="47">
+        <v>16</v>
+      </c>
+      <c r="D17" s="47">
+        <v>0</v>
+      </c>
+      <c r="E17" s="47">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F17" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G17" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H17" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="15">
+      <c r="A18" s="25">
+        <v>193011030</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="48">
+        <v>21</v>
+      </c>
+      <c r="D18" s="48">
+        <v>8</v>
+      </c>
+      <c r="E18" s="47">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="F18" s="27">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G18" s="29">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H18" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="15">
+      <c r="A19" s="25">
+        <v>193012069</v>
+      </c>
+      <c r="B19" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="47">
+        <v>16</v>
+      </c>
+      <c r="D19" s="47">
+        <v>11</v>
+      </c>
+      <c r="E19" s="47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F19" s="27">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="G19" s="29">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="H19" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" ht="15">
+      <c r="A20" s="25">
+        <v>193014003</v>
+      </c>
+      <c r="B20" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="47">
+        <v>21</v>
+      </c>
+      <c r="D20" s="47">
+        <v>4</v>
+      </c>
+      <c r="E20" s="47">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F20" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G20" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H20" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" ht="15">
+      <c r="A21" s="25">
+        <v>193014005</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="47">
+        <v>21</v>
+      </c>
+      <c r="D21" s="47">
+        <v>1</v>
+      </c>
+      <c r="E21" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F21" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G21" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H21" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="15">
+      <c r="A22" s="25">
+        <v>193014007</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="47">
+        <v>21</v>
+      </c>
+      <c r="D22" s="47">
+        <v>7</v>
+      </c>
+      <c r="E22" s="47">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F22" s="27">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G22" s="29">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H22" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" ht="15">
+      <c r="A23" s="25">
+        <v>193014009</v>
+      </c>
+      <c r="B23" s="26" t="s">
+        <v>27</v>
+      </c>
+      <c r="C23" s="47">
+        <v>21</v>
+      </c>
+      <c r="D23" s="47">
+        <v>1</v>
+      </c>
+      <c r="E23" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F23" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G23" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H23" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="15">
+      <c r="A24" s="25">
+        <v>193014010</v>
+      </c>
+      <c r="B24" s="26" t="s">
+        <v>28</v>
+      </c>
+      <c r="C24" s="47">
+        <v>21</v>
+      </c>
+      <c r="D24" s="47">
+        <v>3</v>
+      </c>
+      <c r="E24" s="47">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F24" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G24" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H24" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" ht="15">
+      <c r="A25" s="25">
+        <v>193014015</v>
+      </c>
+      <c r="B25" s="26" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="47">
+        <v>21</v>
+      </c>
+      <c r="D25" s="48">
+        <v>16</v>
+      </c>
+      <c r="E25" s="47">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="F25" s="27">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="G25" s="29">
+        <f t="shared" si="2"/>
+        <v>30</v>
+      </c>
+      <c r="H25" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" ht="15">
+      <c r="A26" s="25">
+        <v>193014016</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="47">
+        <v>21</v>
+      </c>
+      <c r="D26" s="48">
+        <v>18</v>
+      </c>
+      <c r="E26" s="47">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="F26" s="27">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="G26" s="29">
+        <f t="shared" si="2"/>
+        <v>20</v>
+      </c>
+      <c r="H26" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" ht="15">
+      <c r="A27" s="25">
+        <v>193014019</v>
+      </c>
+      <c r="B27" s="26" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="47">
+        <v>21</v>
+      </c>
+      <c r="D27" s="47">
+        <v>5</v>
+      </c>
+      <c r="E27" s="47">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F27" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G27" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H27" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" ht="15">
+      <c r="A28" s="25">
+        <v>193014026</v>
+      </c>
+      <c r="B28" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="C28" s="47">
+        <v>21</v>
+      </c>
+      <c r="D28" s="47">
+        <v>2</v>
+      </c>
+      <c r="E28" s="47">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F28" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G28" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H28" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="15">
+      <c r="A29" s="25">
+        <v>193014030</v>
+      </c>
+      <c r="B29" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="C29" s="47">
+        <v>21</v>
+      </c>
+      <c r="D29" s="47">
+        <v>3</v>
+      </c>
+      <c r="E29" s="47">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F29" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G29" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H29" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" ht="15">
+      <c r="A30" s="25">
+        <v>193014032</v>
+      </c>
+      <c r="B30" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="47">
+        <v>21</v>
+      </c>
+      <c r="D30" s="48">
+        <v>21</v>
+      </c>
+      <c r="E30" s="47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="F30" s="27">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G30" s="29">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H30" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>F</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="15">
+      <c r="A31" s="25">
+        <v>193014033</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="C31" s="47">
+        <v>21</v>
+      </c>
+      <c r="D31" s="47">
+        <v>2</v>
+      </c>
+      <c r="E31" s="47">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F31" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G31" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H31" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" ht="15">
+      <c r="A32" s="25">
+        <v>193014035</v>
+      </c>
+      <c r="B32" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="47">
+        <v>21</v>
+      </c>
+      <c r="D32" s="47">
+        <v>0</v>
+      </c>
+      <c r="E32" s="47">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F32" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G32" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H32" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" ht="15">
+      <c r="A33" s="25">
+        <v>193014036</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C33" s="47">
+        <v>21</v>
+      </c>
+      <c r="D33" s="47">
+        <v>1</v>
+      </c>
+      <c r="E33" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F33" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G33" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H33" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="15">
+      <c r="A34" s="25">
+        <v>193014040</v>
+      </c>
+      <c r="B34" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="C34" s="47">
+        <v>21</v>
+      </c>
+      <c r="D34" s="47">
+        <v>1</v>
+      </c>
+      <c r="E34" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F34" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G34" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H34" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" ht="15">
+      <c r="A35" s="25">
+        <v>193014042</v>
+      </c>
+      <c r="B35" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="C35" s="47">
+        <v>21</v>
+      </c>
+      <c r="D35" s="47">
+        <v>2</v>
+      </c>
+      <c r="E35" s="47">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F35" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G35" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H35" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="15">
+      <c r="A36" s="25">
+        <v>193014048</v>
+      </c>
+      <c r="B36" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="C36" s="47">
+        <v>21</v>
+      </c>
+      <c r="D36" s="47">
+        <v>3</v>
+      </c>
+      <c r="E36" s="47">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F36" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G36" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H36" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" ht="15">
+      <c r="A37" s="25">
+        <v>193014050</v>
+      </c>
+      <c r="B37" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="C37" s="47">
+        <v>21</v>
+      </c>
+      <c r="D37" s="47">
+        <v>4</v>
+      </c>
+      <c r="E37" s="47">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F37" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G37" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H37" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="15">
+      <c r="A38" s="25">
+        <v>193014052</v>
+      </c>
+      <c r="B38" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" s="47">
+        <v>21</v>
+      </c>
+      <c r="D38" s="47">
+        <v>0</v>
+      </c>
+      <c r="E38" s="47">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="F38" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G38" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H38" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="15">
+      <c r="A39" s="25">
+        <v>193014053</v>
+      </c>
+      <c r="B39" s="26" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="47">
+        <v>21</v>
+      </c>
+      <c r="D39" s="47">
+        <v>4</v>
+      </c>
+      <c r="E39" s="47">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="F39" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G39" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H39" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" ht="15">
+      <c r="A40" s="25">
+        <v>193014055</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="C40" s="47">
+        <v>21</v>
+      </c>
+      <c r="D40" s="47">
+        <v>1</v>
+      </c>
+      <c r="E40" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F40" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G40" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H40" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15">
+      <c r="A41" s="25">
+        <v>193014056</v>
+      </c>
+      <c r="B41" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C41" s="47">
+        <v>21</v>
+      </c>
+      <c r="D41" s="47">
+        <v>2</v>
+      </c>
+      <c r="E41" s="47">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F41" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G41" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H41" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" ht="15">
+      <c r="A42" s="25">
+        <v>193014060</v>
+      </c>
+      <c r="B42" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="47">
+        <v>21</v>
+      </c>
+      <c r="D42" s="47">
+        <v>1</v>
+      </c>
+      <c r="E42" s="47">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F42" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G42" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H42" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" ht="15">
+      <c r="A43" s="25">
+        <v>193014061</v>
+      </c>
+      <c r="B43" s="26" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="47">
+        <v>21</v>
+      </c>
+      <c r="D43" s="47">
+        <v>3</v>
+      </c>
+      <c r="E43" s="47">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="F43" s="27">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="G43" s="29">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="H43" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="15">
+      <c r="A44" s="25">
+        <v>193014062</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="47">
+        <v>21</v>
+      </c>
+      <c r="D44" s="47">
+        <v>7</v>
+      </c>
+      <c r="E44" s="47">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="F44" s="27">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="G44" s="29">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="H44" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>B</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" ht="15">
+      <c r="A45" s="25">
+        <v>193014064</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="C45" s="47">
+        <v>21</v>
+      </c>
+      <c r="D45" s="47">
+        <v>6</v>
+      </c>
+      <c r="E45" s="47">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="F45" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G45" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H45" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" ht="15">
+      <c r="A46" s="25">
+        <v>193014065</v>
+      </c>
+      <c r="B46" s="26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C46" s="47">
+        <v>21</v>
+      </c>
+      <c r="D46" s="47">
+        <v>2</v>
+      </c>
+      <c r="E46" s="47">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="F46" s="27">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G46" s="29">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H46" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" ht="15">
+      <c r="A47" s="25">
+        <v>193014067</v>
+      </c>
+      <c r="B47" s="26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C47" s="47">
+        <v>21</v>
+      </c>
+      <c r="D47" s="47">
+        <v>5</v>
+      </c>
+      <c r="E47" s="47">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="F47" s="27">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="G47" s="29">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="H47" s="30" t="str">
+        <f t="shared" si="3"/>
+        <v>A-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="15.75" thickBot="1">
+      <c r="A48" s="32">
+        <v>193014069</v>
+      </c>
+      <c r="B48" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="C48" s="15">
+        <v>21</v>
+      </c>
+      <c r="D48" s="15">
+        <v>1</v>
+      </c>
+      <c r="E48" s="15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="F48" s="16">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="G48" s="21">
+        <f t="shared" si="2"/>
+        <v>100</v>
+      </c>
+      <c r="H48" s="33" t="str">
+        <f t="shared" si="3"/>
+        <v>A+</v>
+      </c>
+    </row>
+    <row r="49" spans="6:6" ht="14.25">
+      <c r="F49" s="27">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C2:E48">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+      <formula>#REF!</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H2:H48">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:L1001"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2:J48"/>
     </sheetView>
   </sheetViews>
@@ -7334,17 +8907,17 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G48">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="1" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7353,7 +8926,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J48"/>
   <sheetViews>
@@ -9014,12 +10587,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="19" priority="3" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9027,7 +10600,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L48"/>
   <sheetViews>
@@ -11107,7 +12680,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:N48"/>
   <sheetViews>
@@ -13287,22 +14860,22 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThan">
       <formula>$D$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThan">
       <formula>$F$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G48">
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="greaterThan">
       <formula>$H$2</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I48">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="14" priority="1" operator="greaterThan">
       <formula>$J$2</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13311,12 +14884,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:J49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C49" sqref="C49"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -14829,27 +16402,27 @@
   </sheetData>
   <phoneticPr fontId="9" type="noConversion"/>
   <conditionalFormatting sqref="C2:C48">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D48">
-    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="7" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E48">
-    <cfRule type="cellIs" dxfId="2" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F48">
-    <cfRule type="cellIs" dxfId="1" priority="9" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="greaterThan">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J48">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14857,7 +16430,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G49"/>
   <sheetViews>

</xml_diff>